<commit_message>
Updated project manager book.
</commit_message>
<xml_diff>
--- a/data/docs/Project Manager Report Book.xlsx
+++ b/data/docs/Project Manager Report Book.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Ampps\www\video-player\data\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22845E61-4D35-4880-BCB0-6C6A456271D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C064D83E-887D-4D11-914F-3CEDC9D52B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feb 2025 01-15" sheetId="45818" r:id="rId1"/>
+    <sheet name="Feb 2025 16-28" sheetId="45819" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Feb 2025 01-15'!$A$2:$U$35</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="54">
   <si>
     <t>Major Tasks</t>
   </si>
@@ -200,6 +201,36 @@
   </si>
   <si>
     <t>I hope to have our site outward-facing and publicly accessible from anywhere on the Internet by the end of the semester. I think we can accomplish that.</t>
+  </si>
+  <si>
+    <t>Date: 02/28/25</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>Accounts/Profile/Login Page</t>
+  </si>
+  <si>
+    <t>Hosting/Domain for Internet access</t>
+  </si>
+  <si>
+    <t>Improvements to UI background for easier viewing (Hunter). Began implementing basic functionality of the the profile page (Ashton).</t>
+  </si>
+  <si>
+    <t>Comments table</t>
+  </si>
+  <si>
+    <t>Likes/dislikes</t>
+  </si>
+  <si>
+    <t>Still need to expand video uploading to upload other formats (Zach). Still tweaking various UI elements (Logan). Researching how to get website hosted for public access (Mikel).</t>
+  </si>
+  <si>
+    <t>We're stalled a little bit, not sure where to go next with the project until the databases are set up properly. There's a minor bug with the sessions, session not activated if login not</t>
+  </si>
+  <si>
+    <t>accessed from the index.html page. It's about time to find a way to get the site outward-facing to the Internet, instead of just being a local network app.</t>
   </si>
 </sst>
 </file>
@@ -306,7 +337,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="52">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -967,13 +998,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="hair">
+        <color indexed="22"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -1223,6 +1269,90 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1256,88 +1386,21 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="52" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="39" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="26" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1346,7 +1409,151 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Project Matrix" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="33">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="10"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="42"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="43"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="10"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="42"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="43"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="10"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="42"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="43"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="10"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="42"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="43"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="10"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="43"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="42"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1694,6 +1901,203 @@
         <a:xfrm>
           <a:off x="4095750" y="5867400"/>
           <a:ext cx="1009650" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="0" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="r" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>Target Dates</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Text Box 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1CCE568-E3F8-49E1-A66C-879A9F833616}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="971550" y="4286250"/>
+          <a:ext cx="2019300" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>Major Tasks</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Text Box 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4276F7BF-56DB-428A-A1A0-060AF60ACA13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="647700" y="5048250"/>
+          <a:ext cx="2647950" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>Summary &amp; Forecast</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1276350</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Text Box 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C7C9695-09E7-4D18-902E-145F1679E2FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2905125" y="4286250"/>
+          <a:ext cx="1009650" cy="971550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2084,8 +2488,8 @@
   </sheetPr>
   <dimension ref="A1:Y40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="73" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="73" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2138,26 +2542,26 @@
       <c r="Y2" s="14"/>
     </row>
     <row r="3" spans="1:25" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="77"/>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="80" t="s">
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="101" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="80"/>
-      <c r="O3" s="80"/>
-      <c r="P3" s="80"/>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
+      <c r="O3" s="101"/>
+      <c r="P3" s="101"/>
       <c r="Q3" s="66"/>
       <c r="R3" s="66"/>
       <c r="S3" s="66"/>
@@ -2168,22 +2572,22 @@
       <c r="Y3" s="14"/>
     </row>
     <row r="4" spans="1:25" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="78"/>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
+      <c r="A4" s="99"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="102"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="102"/>
+      <c r="N4" s="102"/>
+      <c r="O4" s="102"/>
+      <c r="P4" s="102"/>
       <c r="Q4" s="68"/>
       <c r="R4" s="68"/>
       <c r="S4" s="68"/>
@@ -2200,27 +2604,27 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="82" t="s">
+      <c r="E5" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="84"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="86" t="s">
+      <c r="F5" s="104"/>
+      <c r="G5" s="104"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="104"/>
+      <c r="J5" s="104"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="104"/>
+      <c r="N5" s="105"/>
+      <c r="O5" s="105"/>
+      <c r="P5" s="106"/>
+      <c r="Q5" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="R5" s="83"/>
-      <c r="S5" s="83"/>
-      <c r="T5" s="83"/>
-      <c r="U5" s="85"/>
+      <c r="R5" s="104"/>
+      <c r="S5" s="104"/>
+      <c r="T5" s="104"/>
+      <c r="U5" s="106"/>
       <c r="W5" s="21"/>
       <c r="X5" s="22"/>
       <c r="Y5" s="22"/>
@@ -2912,55 +3316,55 @@
       <c r="B26" s="54"/>
       <c r="C26" s="55"/>
       <c r="D26" s="55"/>
-      <c r="E26" s="106" t="s">
+      <c r="E26" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="87" t="s">
+      <c r="F26" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="87" t="s">
+      <c r="G26" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="H26" s="87" t="s">
+      <c r="H26" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="I26" s="87" t="s">
+      <c r="I26" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="J26" s="87" t="s">
+      <c r="J26" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="K26" s="87" t="s">
+      <c r="K26" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="L26" s="87" t="s">
+      <c r="L26" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="M26" s="87" t="s">
+      <c r="M26" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="N26" s="87" t="s">
+      <c r="N26" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="O26" s="87" t="s">
+      <c r="O26" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="P26" s="97" t="s">
+      <c r="P26" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="Q26" s="104" t="s">
+      <c r="Q26" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="R26" s="95" t="s">
+      <c r="R26" s="82" t="s">
         <v>20</v>
       </c>
-      <c r="S26" s="95" t="s">
+      <c r="S26" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="T26" s="95" t="s">
+      <c r="T26" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="U26" s="102" t="s">
+      <c r="U26" s="91" t="s">
         <v>31</v>
       </c>
       <c r="W26" s="31"/>
@@ -2972,23 +3376,23 @@
       <c r="B27" s="56"/>
       <c r="C27" s="55"/>
       <c r="D27" s="55"/>
-      <c r="E27" s="106"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="87"/>
-      <c r="J27" s="87"/>
-      <c r="K27" s="87"/>
-      <c r="L27" s="87"/>
-      <c r="M27" s="87"/>
-      <c r="N27" s="87"/>
-      <c r="O27" s="87"/>
-      <c r="P27" s="97"/>
-      <c r="Q27" s="104"/>
-      <c r="R27" s="95"/>
-      <c r="S27" s="95"/>
-      <c r="T27" s="95"/>
-      <c r="U27" s="102"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="84"/>
+      <c r="H27" s="84"/>
+      <c r="I27" s="84"/>
+      <c r="J27" s="84"/>
+      <c r="K27" s="84"/>
+      <c r="L27" s="84"/>
+      <c r="M27" s="84"/>
+      <c r="N27" s="84"/>
+      <c r="O27" s="84"/>
+      <c r="P27" s="86"/>
+      <c r="Q27" s="93"/>
+      <c r="R27" s="82"/>
+      <c r="S27" s="82"/>
+      <c r="T27" s="82"/>
+      <c r="U27" s="91"/>
       <c r="W27" s="31"/>
       <c r="X27" s="32"/>
       <c r="Y27" s="32"/>
@@ -2998,23 +3402,23 @@
       <c r="B28" s="56"/>
       <c r="C28" s="55"/>
       <c r="D28" s="55"/>
-      <c r="E28" s="106"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="87"/>
-      <c r="H28" s="87"/>
-      <c r="I28" s="87"/>
-      <c r="J28" s="87"/>
-      <c r="K28" s="87"/>
-      <c r="L28" s="87"/>
-      <c r="M28" s="87"/>
-      <c r="N28" s="87"/>
-      <c r="O28" s="87"/>
-      <c r="P28" s="97"/>
-      <c r="Q28" s="104"/>
-      <c r="R28" s="95"/>
-      <c r="S28" s="95"/>
-      <c r="T28" s="95"/>
-      <c r="U28" s="102"/>
+      <c r="E28" s="95"/>
+      <c r="F28" s="84"/>
+      <c r="G28" s="84"/>
+      <c r="H28" s="84"/>
+      <c r="I28" s="84"/>
+      <c r="J28" s="84"/>
+      <c r="K28" s="84"/>
+      <c r="L28" s="84"/>
+      <c r="M28" s="84"/>
+      <c r="N28" s="84"/>
+      <c r="O28" s="84"/>
+      <c r="P28" s="86"/>
+      <c r="Q28" s="93"/>
+      <c r="R28" s="82"/>
+      <c r="S28" s="82"/>
+      <c r="T28" s="82"/>
+      <c r="U28" s="91"/>
       <c r="W28" s="31"/>
       <c r="X28" s="32"/>
       <c r="Y28" s="32"/>
@@ -3024,23 +3428,23 @@
       <c r="B29" s="57"/>
       <c r="C29" s="55"/>
       <c r="D29" s="55"/>
-      <c r="E29" s="106"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
-      <c r="H29" s="87"/>
-      <c r="I29" s="87"/>
-      <c r="J29" s="87"/>
-      <c r="K29" s="87"/>
-      <c r="L29" s="87"/>
-      <c r="M29" s="87"/>
-      <c r="N29" s="87"/>
-      <c r="O29" s="87"/>
-      <c r="P29" s="97"/>
-      <c r="Q29" s="104"/>
-      <c r="R29" s="95"/>
-      <c r="S29" s="95"/>
-      <c r="T29" s="95"/>
-      <c r="U29" s="102"/>
+      <c r="E29" s="95"/>
+      <c r="F29" s="84"/>
+      <c r="G29" s="84"/>
+      <c r="H29" s="84"/>
+      <c r="I29" s="84"/>
+      <c r="J29" s="84"/>
+      <c r="K29" s="84"/>
+      <c r="L29" s="84"/>
+      <c r="M29" s="84"/>
+      <c r="N29" s="84"/>
+      <c r="O29" s="84"/>
+      <c r="P29" s="86"/>
+      <c r="Q29" s="93"/>
+      <c r="R29" s="82"/>
+      <c r="S29" s="82"/>
+      <c r="T29" s="82"/>
+      <c r="U29" s="91"/>
       <c r="X29" s="32"/>
       <c r="Y29" s="32"/>
     </row>
@@ -3049,23 +3453,23 @@
       <c r="B30" s="54"/>
       <c r="C30" s="55"/>
       <c r="D30" s="55"/>
-      <c r="E30" s="106"/>
-      <c r="F30" s="87"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="87"/>
-      <c r="I30" s="87"/>
-      <c r="J30" s="87"/>
-      <c r="K30" s="87"/>
-      <c r="L30" s="87"/>
-      <c r="M30" s="87"/>
-      <c r="N30" s="87"/>
-      <c r="O30" s="87"/>
-      <c r="P30" s="97"/>
-      <c r="Q30" s="104"/>
-      <c r="R30" s="95"/>
-      <c r="S30" s="95"/>
-      <c r="T30" s="95"/>
-      <c r="U30" s="102"/>
+      <c r="E30" s="95"/>
+      <c r="F30" s="84"/>
+      <c r="G30" s="84"/>
+      <c r="H30" s="84"/>
+      <c r="I30" s="84"/>
+      <c r="J30" s="84"/>
+      <c r="K30" s="84"/>
+      <c r="L30" s="84"/>
+      <c r="M30" s="84"/>
+      <c r="N30" s="84"/>
+      <c r="O30" s="84"/>
+      <c r="P30" s="86"/>
+      <c r="Q30" s="93"/>
+      <c r="R30" s="82"/>
+      <c r="S30" s="82"/>
+      <c r="T30" s="82"/>
+      <c r="U30" s="91"/>
       <c r="X30" s="32"/>
       <c r="Y30" s="32"/>
     </row>
@@ -3074,126 +3478,126 @@
       <c r="B31" s="58"/>
       <c r="C31" s="55"/>
       <c r="D31" s="55"/>
-      <c r="E31" s="107"/>
-      <c r="F31" s="88"/>
-      <c r="G31" s="88"/>
-      <c r="H31" s="88"/>
-      <c r="I31" s="88"/>
-      <c r="J31" s="88"/>
-      <c r="K31" s="88"/>
-      <c r="L31" s="88"/>
-      <c r="M31" s="88"/>
-      <c r="N31" s="88"/>
-      <c r="O31" s="88"/>
-      <c r="P31" s="98"/>
-      <c r="Q31" s="105"/>
-      <c r="R31" s="96"/>
-      <c r="S31" s="96"/>
-      <c r="T31" s="96"/>
-      <c r="U31" s="103"/>
+      <c r="E31" s="96"/>
+      <c r="F31" s="85"/>
+      <c r="G31" s="85"/>
+      <c r="H31" s="85"/>
+      <c r="I31" s="85"/>
+      <c r="J31" s="85"/>
+      <c r="K31" s="85"/>
+      <c r="L31" s="85"/>
+      <c r="M31" s="85"/>
+      <c r="N31" s="85"/>
+      <c r="O31" s="85"/>
+      <c r="P31" s="87"/>
+      <c r="Q31" s="94"/>
+      <c r="R31" s="83"/>
+      <c r="S31" s="83"/>
+      <c r="T31" s="83"/>
+      <c r="U31" s="92"/>
       <c r="W31" s="21"/>
       <c r="X31" s="21"/>
       <c r="Y31" s="21"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A32" s="99" t="s">
+      <c r="A32" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="100"/>
-      <c r="C32" s="100"/>
-      <c r="D32" s="100"/>
-      <c r="E32" s="100"/>
-      <c r="F32" s="100"/>
-      <c r="G32" s="100"/>
-      <c r="H32" s="100"/>
-      <c r="I32" s="100"/>
-      <c r="J32" s="100"/>
-      <c r="K32" s="100"/>
-      <c r="L32" s="100"/>
-      <c r="M32" s="100"/>
-      <c r="N32" s="100"/>
-      <c r="O32" s="100"/>
-      <c r="P32" s="100"/>
-      <c r="Q32" s="100"/>
-      <c r="R32" s="100"/>
-      <c r="S32" s="100"/>
-      <c r="T32" s="100"/>
-      <c r="U32" s="101"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="89"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="89"/>
+      <c r="G32" s="89"/>
+      <c r="H32" s="89"/>
+      <c r="I32" s="89"/>
+      <c r="J32" s="89"/>
+      <c r="K32" s="89"/>
+      <c r="L32" s="89"/>
+      <c r="M32" s="89"/>
+      <c r="N32" s="89"/>
+      <c r="O32" s="89"/>
+      <c r="P32" s="89"/>
+      <c r="Q32" s="89"/>
+      <c r="R32" s="89"/>
+      <c r="S32" s="89"/>
+      <c r="T32" s="89"/>
+      <c r="U32" s="90"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A33" s="89" t="s">
+      <c r="A33" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="90"/>
-      <c r="C33" s="90"/>
-      <c r="D33" s="90"/>
-      <c r="E33" s="90"/>
-      <c r="F33" s="90"/>
-      <c r="G33" s="90"/>
-      <c r="H33" s="90"/>
-      <c r="I33" s="90"/>
-      <c r="J33" s="90"/>
-      <c r="K33" s="90"/>
-      <c r="L33" s="90"/>
-      <c r="M33" s="90"/>
-      <c r="N33" s="90"/>
-      <c r="O33" s="90"/>
-      <c r="P33" s="90"/>
-      <c r="Q33" s="90"/>
-      <c r="R33" s="90"/>
-      <c r="S33" s="90"/>
-      <c r="T33" s="90"/>
-      <c r="U33" s="91"/>
+      <c r="B33" s="77"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="77"/>
+      <c r="H33" s="77"/>
+      <c r="I33" s="77"/>
+      <c r="J33" s="77"/>
+      <c r="K33" s="77"/>
+      <c r="L33" s="77"/>
+      <c r="M33" s="77"/>
+      <c r="N33" s="77"/>
+      <c r="O33" s="77"/>
+      <c r="P33" s="77"/>
+      <c r="Q33" s="77"/>
+      <c r="R33" s="77"/>
+      <c r="S33" s="77"/>
+      <c r="T33" s="77"/>
+      <c r="U33" s="78"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A34" s="89" t="s">
+      <c r="A34" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="90"/>
-      <c r="C34" s="90"/>
-      <c r="D34" s="90"/>
-      <c r="E34" s="90"/>
-      <c r="F34" s="90"/>
-      <c r="G34" s="90"/>
-      <c r="H34" s="90"/>
-      <c r="I34" s="90"/>
-      <c r="J34" s="90"/>
-      <c r="K34" s="90"/>
-      <c r="L34" s="90"/>
-      <c r="M34" s="90"/>
-      <c r="N34" s="90"/>
-      <c r="O34" s="90"/>
-      <c r="P34" s="90"/>
-      <c r="Q34" s="90"/>
-      <c r="R34" s="90"/>
-      <c r="S34" s="90"/>
-      <c r="T34" s="90"/>
-      <c r="U34" s="91"/>
+      <c r="B34" s="77"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="77"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
+      <c r="L34" s="77"/>
+      <c r="M34" s="77"/>
+      <c r="N34" s="77"/>
+      <c r="O34" s="77"/>
+      <c r="P34" s="77"/>
+      <c r="Q34" s="77"/>
+      <c r="R34" s="77"/>
+      <c r="S34" s="77"/>
+      <c r="T34" s="77"/>
+      <c r="U34" s="78"/>
     </row>
     <row r="35" spans="1:25" s="18" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="92" t="s">
+      <c r="A35" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="93"/>
-      <c r="C35" s="93"/>
-      <c r="D35" s="93"/>
-      <c r="E35" s="93"/>
-      <c r="F35" s="93"/>
-      <c r="G35" s="93"/>
-      <c r="H35" s="93"/>
-      <c r="I35" s="93"/>
-      <c r="J35" s="93"/>
-      <c r="K35" s="93"/>
-      <c r="L35" s="93"/>
-      <c r="M35" s="93"/>
-      <c r="N35" s="93"/>
-      <c r="O35" s="93"/>
-      <c r="P35" s="93"/>
-      <c r="Q35" s="93"/>
-      <c r="R35" s="93"/>
-      <c r="S35" s="93"/>
-      <c r="T35" s="93"/>
-      <c r="U35" s="94"/>
+      <c r="B35" s="80"/>
+      <c r="C35" s="80"/>
+      <c r="D35" s="80"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="80"/>
+      <c r="G35" s="80"/>
+      <c r="H35" s="80"/>
+      <c r="I35" s="80"/>
+      <c r="J35" s="80"/>
+      <c r="K35" s="80"/>
+      <c r="L35" s="80"/>
+      <c r="M35" s="80"/>
+      <c r="N35" s="80"/>
+      <c r="O35" s="80"/>
+      <c r="P35" s="80"/>
+      <c r="Q35" s="80"/>
+      <c r="R35" s="80"/>
+      <c r="S35" s="80"/>
+      <c r="T35" s="80"/>
+      <c r="U35" s="81"/>
       <c r="W35" s="21"/>
       <c r="X35" s="22"/>
       <c r="Y35" s="22"/>
@@ -3275,6 +3679,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="E3:P4"/>
+    <mergeCell ref="E5:P5"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="F26:F31"/>
+    <mergeCell ref="G26:G31"/>
+    <mergeCell ref="N26:N31"/>
+    <mergeCell ref="I26:I31"/>
+    <mergeCell ref="J26:J31"/>
     <mergeCell ref="A34:U34"/>
     <mergeCell ref="A35:U35"/>
     <mergeCell ref="T26:T31"/>
@@ -3291,80 +3704,71 @@
     <mergeCell ref="Q26:Q31"/>
     <mergeCell ref="K26:K31"/>
     <mergeCell ref="E26:E31"/>
-    <mergeCell ref="A3:D4"/>
-    <mergeCell ref="E3:P4"/>
-    <mergeCell ref="E5:P5"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="F26:F31"/>
-    <mergeCell ref="G26:G31"/>
-    <mergeCell ref="N26:N31"/>
-    <mergeCell ref="I26:I31"/>
-    <mergeCell ref="J26:J31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D38:E38 I38:Y38">
-    <cfRule type="cellIs" dxfId="17" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="26" stopIfTrue="1" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="27" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="27" stopIfTrue="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="28" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="28" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:G6 I6:K6 M6:P6 G7:N7 P7 G8:L8 E9:F9 J9:L9 E10:G10 I10:M10 O10:P10 E11:J11 E12:G12 K12 E13:H13 J13:N13 P13 N14:P14 E14:I15 M15:O15 E16:J16 L16:P16 E17:I17 K17:P17 E18:P25">
-    <cfRule type="cellIs" dxfId="14" priority="29" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="29" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="30" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="30" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="31" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="31" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="11" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="13" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="14" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="15" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="8" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="10" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="11" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="12" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11:P12">
-    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8:P9">
-    <cfRule type="cellIs" dxfId="2" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="16" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="18" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3375,4 +3779,1284 @@
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52089AA5-E353-4911-A982-D49FBFB6A530}">
+  <dimension ref="A1:Y40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.625" style="1" customWidth="1"/>
+    <col min="5" max="16" width="5" style="1" customWidth="1"/>
+    <col min="17" max="20" width="4.125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="4.5" style="1" customWidth="1"/>
+    <col min="22" max="22" width="2.625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="6.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:25" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="W2" s="13"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+    </row>
+    <row r="3" spans="1:25" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="97" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="98"/>
+      <c r="C3" s="98"/>
+      <c r="D3" s="98"/>
+      <c r="E3" s="101" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="101"/>
+      <c r="G3" s="101"/>
+      <c r="H3" s="101"/>
+      <c r="I3" s="101"/>
+      <c r="J3" s="101"/>
+      <c r="K3" s="101"/>
+      <c r="L3" s="101"/>
+      <c r="M3" s="101"/>
+      <c r="N3" s="101"/>
+      <c r="O3" s="101"/>
+      <c r="P3" s="101"/>
+      <c r="Q3" s="66"/>
+      <c r="R3" s="66"/>
+      <c r="S3" s="66"/>
+      <c r="T3" s="66"/>
+      <c r="U3" s="67"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+    </row>
+    <row r="4" spans="1:25" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="99"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="102"/>
+      <c r="K4" s="102"/>
+      <c r="L4" s="102"/>
+      <c r="M4" s="102"/>
+      <c r="N4" s="102"/>
+      <c r="O4" s="102"/>
+      <c r="P4" s="102"/>
+      <c r="Q4" s="68"/>
+      <c r="R4" s="68"/>
+      <c r="S4" s="68"/>
+      <c r="T4" s="68"/>
+      <c r="U4" s="69"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+    </row>
+    <row r="5" spans="1:25" s="18" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="103" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="104"/>
+      <c r="G5" s="104"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="104"/>
+      <c r="J5" s="104"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="104"/>
+      <c r="N5" s="105"/>
+      <c r="O5" s="105"/>
+      <c r="P5" s="106"/>
+      <c r="Q5" s="107" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" s="104"/>
+      <c r="S5" s="104"/>
+      <c r="T5" s="104"/>
+      <c r="U5" s="106"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="22"/>
+      <c r="Y5" s="22"/>
+    </row>
+    <row r="6" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="24">
+        <v>1</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="70"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S6" s="29"/>
+      <c r="T6" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U6" s="30"/>
+      <c r="W6" s="31"/>
+      <c r="X6" s="32"/>
+      <c r="Y6" s="32"/>
+    </row>
+    <row r="7" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="33">
+        <v>2</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="O7" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S7" s="40"/>
+      <c r="T7" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U7" s="41"/>
+      <c r="W7" s="31"/>
+      <c r="X7" s="32"/>
+      <c r="Y7" s="32"/>
+    </row>
+    <row r="8" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="33">
+        <v>3</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S8" s="40"/>
+      <c r="T8" s="40"/>
+      <c r="U8" s="41"/>
+      <c r="W8" s="31"/>
+      <c r="X8" s="32"/>
+      <c r="Y8" s="32"/>
+    </row>
+    <row r="9" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="33">
+        <v>4</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="37"/>
+      <c r="I9" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="N9" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="O9" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="T9" s="40"/>
+      <c r="U9" s="41"/>
+      <c r="W9" s="31"/>
+      <c r="X9" s="32"/>
+      <c r="Y9" s="32"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="111"/>
+      <c r="M10" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="O10" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P10" s="111"/>
+      <c r="U10" s="111"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="111"/>
+      <c r="M11" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="O11" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P11" s="111"/>
+      <c r="U11" s="111"/>
+    </row>
+    <row r="12" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="33">
+        <v>4.3</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="37"/>
+      <c r="J12" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" s="37"/>
+      <c r="L12" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="M12" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="N12" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="O12" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="40"/>
+      <c r="T12" s="40"/>
+      <c r="U12" s="41"/>
+      <c r="W12" s="31"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="32"/>
+    </row>
+    <row r="13" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="33">
+        <v>5</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="N13" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="O13" s="37"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="40"/>
+      <c r="T13" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U13" s="41"/>
+      <c r="W13" s="31"/>
+      <c r="X13" s="32"/>
+      <c r="Y13" s="32"/>
+    </row>
+    <row r="14" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="33">
+        <v>6</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="L14" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="37"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="R14" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S14" s="40"/>
+      <c r="T14" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U14" s="41"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="32"/>
+      <c r="Y14" s="32"/>
+    </row>
+    <row r="15" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="33">
+        <v>7</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="R15" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S15" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="T15" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U15" s="75" t="s">
+        <v>4</v>
+      </c>
+      <c r="W15" s="31"/>
+      <c r="X15" s="32"/>
+      <c r="Y15" s="32"/>
+    </row>
+    <row r="16" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="33">
+        <v>8</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="L16" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="M16" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="38"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="40"/>
+      <c r="S16" s="40"/>
+      <c r="T16" s="40"/>
+      <c r="U16" s="75" t="s">
+        <v>4</v>
+      </c>
+      <c r="W16" s="31"/>
+      <c r="X16" s="32"/>
+      <c r="Y16" s="32"/>
+    </row>
+    <row r="17" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="33">
+        <v>9</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="L17" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="T17" s="40"/>
+      <c r="U17" s="41"/>
+      <c r="W17" s="31"/>
+      <c r="X17" s="32"/>
+      <c r="Y17" s="32"/>
+    </row>
+    <row r="18" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="33">
+        <v>10</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="39"/>
+      <c r="R18" s="40"/>
+      <c r="S18" s="40"/>
+      <c r="T18" s="40"/>
+      <c r="U18" s="75" t="s">
+        <v>4</v>
+      </c>
+      <c r="W18" s="31"/>
+      <c r="X18" s="32"/>
+      <c r="Y18" s="32"/>
+    </row>
+    <row r="19" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="33">
+        <v>11</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="73"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="N19" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="O19" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P19" s="108" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="109" t="s">
+        <v>4</v>
+      </c>
+      <c r="R19" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S19" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="T19" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U19" s="75" t="s">
+        <v>4</v>
+      </c>
+      <c r="W19" s="31"/>
+      <c r="X19" s="32"/>
+      <c r="Y19" s="32"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>12</v>
+      </c>
+      <c r="D20" s="111"/>
+      <c r="P20" s="111"/>
+      <c r="U20" s="111"/>
+    </row>
+    <row r="21" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="33">
+        <v>13</v>
+      </c>
+      <c r="B21" s="42"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="41"/>
+      <c r="W21" s="31"/>
+      <c r="X21" s="32"/>
+      <c r="Y21" s="32"/>
+    </row>
+    <row r="22" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="33">
+        <v>14</v>
+      </c>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="39"/>
+      <c r="R22" s="40"/>
+      <c r="S22" s="40"/>
+      <c r="T22" s="40"/>
+      <c r="U22" s="41"/>
+      <c r="W22" s="31"/>
+      <c r="X22" s="32"/>
+      <c r="Y22" s="32"/>
+    </row>
+    <row r="23" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="33">
+        <v>15</v>
+      </c>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="37"/>
+      <c r="O23" s="37"/>
+      <c r="P23" s="38"/>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="40"/>
+      <c r="S23" s="40"/>
+      <c r="T23" s="40"/>
+      <c r="U23" s="41"/>
+      <c r="W23" s="31"/>
+      <c r="X23" s="32"/>
+      <c r="Y23" s="32"/>
+    </row>
+    <row r="24" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="33">
+        <v>16</v>
+      </c>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="37"/>
+      <c r="K24" s="37"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="37"/>
+      <c r="O24" s="37"/>
+      <c r="P24" s="38"/>
+      <c r="Q24" s="39"/>
+      <c r="R24" s="40"/>
+      <c r="S24" s="40"/>
+      <c r="T24" s="40"/>
+      <c r="U24" s="41"/>
+      <c r="W24" s="31"/>
+      <c r="X24" s="32"/>
+      <c r="Y24" s="32"/>
+    </row>
+    <row r="25" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="44">
+        <v>17</v>
+      </c>
+      <c r="B25" s="45"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="48"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="48"/>
+      <c r="O25" s="48"/>
+      <c r="P25" s="49"/>
+      <c r="Q25" s="50"/>
+      <c r="R25" s="51"/>
+      <c r="S25" s="51"/>
+      <c r="T25" s="51"/>
+      <c r="U25" s="52"/>
+      <c r="W25" s="31"/>
+      <c r="X25" s="32"/>
+      <c r="Y25" s="32"/>
+    </row>
+    <row r="26" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="53"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="95" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="84" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="84" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="84" t="s">
+        <v>10</v>
+      </c>
+      <c r="I26" s="84" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" s="84" t="s">
+        <v>12</v>
+      </c>
+      <c r="K26" s="84" t="s">
+        <v>13</v>
+      </c>
+      <c r="L26" s="84" t="s">
+        <v>14</v>
+      </c>
+      <c r="M26" s="84" t="s">
+        <v>15</v>
+      </c>
+      <c r="N26" s="84" t="s">
+        <v>16</v>
+      </c>
+      <c r="O26" s="84" t="s">
+        <v>17</v>
+      </c>
+      <c r="P26" s="86" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q26" s="93" t="s">
+        <v>19</v>
+      </c>
+      <c r="R26" s="82" t="s">
+        <v>20</v>
+      </c>
+      <c r="S26" s="82" t="s">
+        <v>21</v>
+      </c>
+      <c r="T26" s="82" t="s">
+        <v>30</v>
+      </c>
+      <c r="U26" s="91" t="s">
+        <v>31</v>
+      </c>
+      <c r="W26" s="31"/>
+      <c r="X26" s="32"/>
+      <c r="Y26" s="32"/>
+    </row>
+    <row r="27" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="53"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="84"/>
+      <c r="G27" s="84"/>
+      <c r="H27" s="84"/>
+      <c r="I27" s="84"/>
+      <c r="J27" s="84"/>
+      <c r="K27" s="84"/>
+      <c r="L27" s="84"/>
+      <c r="M27" s="84"/>
+      <c r="N27" s="84"/>
+      <c r="O27" s="84"/>
+      <c r="P27" s="86"/>
+      <c r="Q27" s="93"/>
+      <c r="R27" s="82"/>
+      <c r="S27" s="82"/>
+      <c r="T27" s="82"/>
+      <c r="U27" s="91"/>
+      <c r="W27" s="31"/>
+      <c r="X27" s="32"/>
+      <c r="Y27" s="32"/>
+    </row>
+    <row r="28" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="53"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="95"/>
+      <c r="F28" s="84"/>
+      <c r="G28" s="84"/>
+      <c r="H28" s="84"/>
+      <c r="I28" s="84"/>
+      <c r="J28" s="84"/>
+      <c r="K28" s="84"/>
+      <c r="L28" s="84"/>
+      <c r="M28" s="84"/>
+      <c r="N28" s="84"/>
+      <c r="O28" s="84"/>
+      <c r="P28" s="86"/>
+      <c r="Q28" s="93"/>
+      <c r="R28" s="82"/>
+      <c r="S28" s="82"/>
+      <c r="T28" s="82"/>
+      <c r="U28" s="91"/>
+      <c r="W28" s="31"/>
+      <c r="X28" s="32"/>
+      <c r="Y28" s="32"/>
+    </row>
+    <row r="29" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="53"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="95"/>
+      <c r="F29" s="84"/>
+      <c r="G29" s="84"/>
+      <c r="H29" s="84"/>
+      <c r="I29" s="84"/>
+      <c r="J29" s="84"/>
+      <c r="K29" s="84"/>
+      <c r="L29" s="84"/>
+      <c r="M29" s="84"/>
+      <c r="N29" s="84"/>
+      <c r="O29" s="84"/>
+      <c r="P29" s="86"/>
+      <c r="Q29" s="93"/>
+      <c r="R29" s="82"/>
+      <c r="S29" s="82"/>
+      <c r="T29" s="82"/>
+      <c r="U29" s="91"/>
+      <c r="X29" s="32"/>
+      <c r="Y29" s="32"/>
+    </row>
+    <row r="30" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="53"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="95"/>
+      <c r="F30" s="84"/>
+      <c r="G30" s="84"/>
+      <c r="H30" s="84"/>
+      <c r="I30" s="84"/>
+      <c r="J30" s="84"/>
+      <c r="K30" s="84"/>
+      <c r="L30" s="84"/>
+      <c r="M30" s="84"/>
+      <c r="N30" s="84"/>
+      <c r="O30" s="84"/>
+      <c r="P30" s="86"/>
+      <c r="Q30" s="93"/>
+      <c r="R30" s="82"/>
+      <c r="S30" s="82"/>
+      <c r="T30" s="82"/>
+      <c r="U30" s="91"/>
+      <c r="X30" s="32"/>
+      <c r="Y30" s="32"/>
+    </row>
+    <row r="31" spans="1:25" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="53"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="96"/>
+      <c r="F31" s="85"/>
+      <c r="G31" s="85"/>
+      <c r="H31" s="85"/>
+      <c r="I31" s="85"/>
+      <c r="J31" s="85"/>
+      <c r="K31" s="85"/>
+      <c r="L31" s="85"/>
+      <c r="M31" s="85"/>
+      <c r="N31" s="85"/>
+      <c r="O31" s="85"/>
+      <c r="P31" s="87"/>
+      <c r="Q31" s="94"/>
+      <c r="R31" s="83"/>
+      <c r="S31" s="83"/>
+      <c r="T31" s="83"/>
+      <c r="U31" s="92"/>
+      <c r="W31" s="21"/>
+      <c r="X31" s="21"/>
+      <c r="Y31" s="21"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A32" s="110" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="89"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="89"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="89"/>
+      <c r="G32" s="89"/>
+      <c r="H32" s="89"/>
+      <c r="I32" s="89"/>
+      <c r="J32" s="89"/>
+      <c r="K32" s="89"/>
+      <c r="L32" s="89"/>
+      <c r="M32" s="89"/>
+      <c r="N32" s="89"/>
+      <c r="O32" s="89"/>
+      <c r="P32" s="89"/>
+      <c r="Q32" s="89"/>
+      <c r="R32" s="89"/>
+      <c r="S32" s="89"/>
+      <c r="T32" s="89"/>
+      <c r="U32" s="90"/>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A33" s="112" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" s="77"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="77"/>
+      <c r="H33" s="77"/>
+      <c r="I33" s="77"/>
+      <c r="J33" s="77"/>
+      <c r="K33" s="77"/>
+      <c r="L33" s="77"/>
+      <c r="M33" s="77"/>
+      <c r="N33" s="77"/>
+      <c r="O33" s="77"/>
+      <c r="P33" s="77"/>
+      <c r="Q33" s="77"/>
+      <c r="R33" s="77"/>
+      <c r="S33" s="77"/>
+      <c r="T33" s="77"/>
+      <c r="U33" s="78"/>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A34" s="112" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="77"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="77"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="77"/>
+      <c r="K34" s="77"/>
+      <c r="L34" s="77"/>
+      <c r="M34" s="77"/>
+      <c r="N34" s="77"/>
+      <c r="O34" s="77"/>
+      <c r="P34" s="77"/>
+      <c r="Q34" s="77"/>
+      <c r="R34" s="77"/>
+      <c r="S34" s="77"/>
+      <c r="T34" s="77"/>
+      <c r="U34" s="78"/>
+    </row>
+    <row r="35" spans="1:25" s="18" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="79" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="80"/>
+      <c r="C35" s="80"/>
+      <c r="D35" s="80"/>
+      <c r="E35" s="80"/>
+      <c r="F35" s="80"/>
+      <c r="G35" s="80"/>
+      <c r="H35" s="80"/>
+      <c r="I35" s="80"/>
+      <c r="J35" s="80"/>
+      <c r="K35" s="80"/>
+      <c r="L35" s="80"/>
+      <c r="M35" s="80"/>
+      <c r="N35" s="80"/>
+      <c r="O35" s="80"/>
+      <c r="P35" s="80"/>
+      <c r="Q35" s="80"/>
+      <c r="R35" s="80"/>
+      <c r="S35" s="80"/>
+      <c r="T35" s="80"/>
+      <c r="U35" s="81"/>
+      <c r="W35" s="21"/>
+      <c r="X35" s="22"/>
+      <c r="Y35" s="22"/>
+    </row>
+    <row r="36" spans="1:25" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="W36" s="21"/>
+      <c r="X36" s="22"/>
+      <c r="Y36" s="22"/>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="F37" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G37" s="59">
+        <v>152</v>
+      </c>
+      <c r="H37" s="63">
+        <v>153</v>
+      </c>
+      <c r="I37" s="64"/>
+      <c r="J37" s="64"/>
+      <c r="K37" s="60"/>
+      <c r="L37" s="60"/>
+      <c r="M37" s="60"/>
+      <c r="N37" s="60"/>
+      <c r="O37" s="60"/>
+      <c r="P37" s="60"/>
+      <c r="Q37" s="60"/>
+      <c r="R37" s="60"/>
+      <c r="S37" s="60"/>
+      <c r="T37" s="60"/>
+      <c r="U37" s="60"/>
+      <c r="V37" s="60"/>
+      <c r="W37" s="60"/>
+      <c r="X37" s="60"/>
+      <c r="Y37" s="60"/>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="F38" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="H38" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="I38" s="61"/>
+      <c r="J38" s="61"/>
+      <c r="K38" s="61"/>
+      <c r="L38" s="61"/>
+      <c r="M38" s="61"/>
+      <c r="N38" s="61"/>
+      <c r="O38" s="61"/>
+      <c r="P38" s="61"/>
+      <c r="Q38" s="61"/>
+      <c r="R38" s="61"/>
+      <c r="S38" s="61"/>
+      <c r="T38" s="61"/>
+      <c r="U38" s="61"/>
+      <c r="V38" s="61"/>
+      <c r="W38" s="61"/>
+      <c r="X38" s="61"/>
+      <c r="Y38" s="61"/>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+      <c r="Y39" s="1"/>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="W40" s="1"/>
+      <c r="X40" s="1"/>
+      <c r="Y40" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="A33:U33"/>
+    <mergeCell ref="A34:U34"/>
+    <mergeCell ref="A35:U35"/>
+    <mergeCell ref="Q26:Q31"/>
+    <mergeCell ref="R26:R31"/>
+    <mergeCell ref="S26:S31"/>
+    <mergeCell ref="T26:T31"/>
+    <mergeCell ref="U26:U31"/>
+    <mergeCell ref="A32:U32"/>
+    <mergeCell ref="K26:K31"/>
+    <mergeCell ref="L26:L31"/>
+    <mergeCell ref="M26:M31"/>
+    <mergeCell ref="N26:N31"/>
+    <mergeCell ref="O26:O31"/>
+    <mergeCell ref="P26:P31"/>
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="E3:P4"/>
+    <mergeCell ref="E5:P5"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="E26:E31"/>
+    <mergeCell ref="F26:F31"/>
+    <mergeCell ref="G26:G31"/>
+    <mergeCell ref="H26:H31"/>
+    <mergeCell ref="I26:I31"/>
+    <mergeCell ref="J26:J31"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D38:E38 I38:Y38">
+    <cfRule type="cellIs" dxfId="14" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"G"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6:G6 I6:K6 M6:P6 P7 G7:L8 E9:F9 J9:L9 I13:L13 E14:J14 E12:G13 K12 E15:H15 J15:N15 P15 N16:P16 E16:I17 M17:O17 E18:J18 L18:P18 E19:I19 K19:L19 E21:P25 M14:P14 O13:P13 P12">
+    <cfRule type="cellIs" dxfId="11" priority="16" stopIfTrue="1" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="17" stopIfTrue="1" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="18" stopIfTrue="1" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H9">
+    <cfRule type="cellIs" dxfId="8" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N8:P8 P9">
+    <cfRule type="cellIs" dxfId="2" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
(WIP) Implementing profile page API.
</commit_message>
<xml_diff>
--- a/data/docs/Project Manager Report Book.xlsx
+++ b/data/docs/Project Manager Report Book.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Ampps\www\video-player\data\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C064D83E-887D-4D11-914F-3CEDC9D52B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945FEBAE-FAC6-4BAB-8657-7EC76B094158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11235" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feb 2025 01-15" sheetId="45818" r:id="rId1"/>
     <sheet name="Feb 2025 16-28" sheetId="45819" r:id="rId2"/>
+    <sheet name="Mar 2025 01-21" sheetId="45820" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Feb 2025 01-15'!$A$2:$U$35</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="59">
   <si>
     <t>Major Tasks</t>
   </si>
@@ -231,6 +232,21 @@
   </si>
   <si>
     <t>accessed from the index.html page. It's about time to find a way to get the site outward-facing to the Internet, instead of just being a local network app.</t>
+  </si>
+  <si>
+    <t>API</t>
+  </si>
+  <si>
+    <t>Spent spring break attempting to design an API (Mikel).</t>
+  </si>
+  <si>
+    <t>I honestly don't know what everyone else did. I didn't really ask them to do anything, they've been waiting on me to finish the API so they can use it to frontend work.</t>
+  </si>
+  <si>
+    <t>Dockerization</t>
+  </si>
+  <si>
+    <t>I'm not a good project manager. I'm not good at anything.</t>
   </si>
 </sst>
 </file>
@@ -1269,6 +1285,56 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="52" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -1301,14 +1367,6 @@
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="17" fontId="5" fillId="0" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
       <protection locked="0"/>
@@ -1353,53 +1411,11 @@
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="52" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -1409,7 +1425,151 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Project Matrix" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="48">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="10"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="42"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="43"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="10"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="42"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="43"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="10"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="42"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="43"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="10"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="42"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="43"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="10"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="43"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="42"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2135,6 +2295,203 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Text Box 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0434135-1025-4F60-93CE-F7F5CCC1DDD9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="971550" y="4286250"/>
+          <a:ext cx="2019300" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>Major Tasks</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Text Box 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A06AC21C-FD0E-44C0-AE15-D0C3A1B3AEC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="647700" y="5048250"/>
+          <a:ext cx="2647950" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>Summary &amp; Forecast</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1276350</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Text Box 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA882AE1-0206-4712-AE5A-CA4AC09F2887}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2905125" y="4286250"/>
+          <a:ext cx="1009650" cy="971550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="0" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="r" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>Target Dates</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2542,26 +2899,26 @@
       <c r="Y2" s="14"/>
     </row>
     <row r="3" spans="1:25" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="101" t="s">
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="N3" s="101"/>
-      <c r="O3" s="101"/>
-      <c r="P3" s="101"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="83"/>
       <c r="Q3" s="66"/>
       <c r="R3" s="66"/>
       <c r="S3" s="66"/>
@@ -2572,22 +2929,22 @@
       <c r="Y3" s="14"/>
     </row>
     <row r="4" spans="1:25" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="99"/>
-      <c r="B4" s="100"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="102"/>
-      <c r="L4" s="102"/>
-      <c r="M4" s="102"/>
-      <c r="N4" s="102"/>
-      <c r="O4" s="102"/>
-      <c r="P4" s="102"/>
+      <c r="A4" s="81"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="84"/>
+      <c r="L4" s="84"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="84"/>
+      <c r="O4" s="84"/>
+      <c r="P4" s="84"/>
       <c r="Q4" s="68"/>
       <c r="R4" s="68"/>
       <c r="S4" s="68"/>
@@ -2604,27 +2961,27 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="103" t="s">
+      <c r="E5" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="104"/>
-      <c r="G5" s="104"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="104"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="104"/>
-      <c r="N5" s="105"/>
-      <c r="O5" s="105"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="107" t="s">
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="88"/>
+      <c r="Q5" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="R5" s="104"/>
-      <c r="S5" s="104"/>
-      <c r="T5" s="104"/>
-      <c r="U5" s="106"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="86"/>
+      <c r="T5" s="86"/>
+      <c r="U5" s="88"/>
       <c r="W5" s="21"/>
       <c r="X5" s="22"/>
       <c r="Y5" s="22"/>
@@ -3316,55 +3673,55 @@
       <c r="B26" s="54"/>
       <c r="C26" s="55"/>
       <c r="D26" s="55"/>
-      <c r="E26" s="95" t="s">
+      <c r="E26" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="84" t="s">
+      <c r="F26" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="84" t="s">
+      <c r="G26" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="H26" s="84" t="s">
+      <c r="H26" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="I26" s="84" t="s">
+      <c r="I26" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="J26" s="84" t="s">
+      <c r="J26" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="K26" s="84" t="s">
+      <c r="K26" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="L26" s="84" t="s">
+      <c r="L26" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="M26" s="84" t="s">
+      <c r="M26" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="N26" s="84" t="s">
+      <c r="N26" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="O26" s="84" t="s">
+      <c r="O26" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="P26" s="86" t="s">
+      <c r="P26" s="100" t="s">
         <v>18</v>
       </c>
-      <c r="Q26" s="93" t="s">
+      <c r="Q26" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="R26" s="82" t="s">
+      <c r="R26" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="S26" s="82" t="s">
+      <c r="S26" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="T26" s="82" t="s">
+      <c r="T26" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="U26" s="91" t="s">
+      <c r="U26" s="105" t="s">
         <v>31</v>
       </c>
       <c r="W26" s="31"/>
@@ -3376,23 +3733,23 @@
       <c r="B27" s="56"/>
       <c r="C27" s="55"/>
       <c r="D27" s="55"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="84"/>
-      <c r="G27" s="84"/>
-      <c r="H27" s="84"/>
-      <c r="I27" s="84"/>
-      <c r="J27" s="84"/>
-      <c r="K27" s="84"/>
-      <c r="L27" s="84"/>
-      <c r="M27" s="84"/>
-      <c r="N27" s="84"/>
-      <c r="O27" s="84"/>
-      <c r="P27" s="86"/>
-      <c r="Q27" s="93"/>
-      <c r="R27" s="82"/>
-      <c r="S27" s="82"/>
-      <c r="T27" s="82"/>
-      <c r="U27" s="91"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="90"/>
+      <c r="J27" s="90"/>
+      <c r="K27" s="90"/>
+      <c r="L27" s="90"/>
+      <c r="M27" s="90"/>
+      <c r="N27" s="90"/>
+      <c r="O27" s="90"/>
+      <c r="P27" s="100"/>
+      <c r="Q27" s="107"/>
+      <c r="R27" s="98"/>
+      <c r="S27" s="98"/>
+      <c r="T27" s="98"/>
+      <c r="U27" s="105"/>
       <c r="W27" s="31"/>
       <c r="X27" s="32"/>
       <c r="Y27" s="32"/>
@@ -3402,23 +3759,23 @@
       <c r="B28" s="56"/>
       <c r="C28" s="55"/>
       <c r="D28" s="55"/>
-      <c r="E28" s="95"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="84"/>
-      <c r="I28" s="84"/>
-      <c r="J28" s="84"/>
-      <c r="K28" s="84"/>
-      <c r="L28" s="84"/>
-      <c r="M28" s="84"/>
-      <c r="N28" s="84"/>
-      <c r="O28" s="84"/>
-      <c r="P28" s="86"/>
-      <c r="Q28" s="93"/>
-      <c r="R28" s="82"/>
-      <c r="S28" s="82"/>
-      <c r="T28" s="82"/>
-      <c r="U28" s="91"/>
+      <c r="E28" s="109"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="90"/>
+      <c r="H28" s="90"/>
+      <c r="I28" s="90"/>
+      <c r="J28" s="90"/>
+      <c r="K28" s="90"/>
+      <c r="L28" s="90"/>
+      <c r="M28" s="90"/>
+      <c r="N28" s="90"/>
+      <c r="O28" s="90"/>
+      <c r="P28" s="100"/>
+      <c r="Q28" s="107"/>
+      <c r="R28" s="98"/>
+      <c r="S28" s="98"/>
+      <c r="T28" s="98"/>
+      <c r="U28" s="105"/>
       <c r="W28" s="31"/>
       <c r="X28" s="32"/>
       <c r="Y28" s="32"/>
@@ -3428,23 +3785,23 @@
       <c r="B29" s="57"/>
       <c r="C29" s="55"/>
       <c r="D29" s="55"/>
-      <c r="E29" s="95"/>
-      <c r="F29" s="84"/>
-      <c r="G29" s="84"/>
-      <c r="H29" s="84"/>
-      <c r="I29" s="84"/>
-      <c r="J29" s="84"/>
-      <c r="K29" s="84"/>
-      <c r="L29" s="84"/>
-      <c r="M29" s="84"/>
-      <c r="N29" s="84"/>
-      <c r="O29" s="84"/>
-      <c r="P29" s="86"/>
-      <c r="Q29" s="93"/>
-      <c r="R29" s="82"/>
-      <c r="S29" s="82"/>
-      <c r="T29" s="82"/>
-      <c r="U29" s="91"/>
+      <c r="E29" s="109"/>
+      <c r="F29" s="90"/>
+      <c r="G29" s="90"/>
+      <c r="H29" s="90"/>
+      <c r="I29" s="90"/>
+      <c r="J29" s="90"/>
+      <c r="K29" s="90"/>
+      <c r="L29" s="90"/>
+      <c r="M29" s="90"/>
+      <c r="N29" s="90"/>
+      <c r="O29" s="90"/>
+      <c r="P29" s="100"/>
+      <c r="Q29" s="107"/>
+      <c r="R29" s="98"/>
+      <c r="S29" s="98"/>
+      <c r="T29" s="98"/>
+      <c r="U29" s="105"/>
       <c r="X29" s="32"/>
       <c r="Y29" s="32"/>
     </row>
@@ -3453,23 +3810,23 @@
       <c r="B30" s="54"/>
       <c r="C30" s="55"/>
       <c r="D30" s="55"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="84"/>
-      <c r="G30" s="84"/>
-      <c r="H30" s="84"/>
-      <c r="I30" s="84"/>
-      <c r="J30" s="84"/>
-      <c r="K30" s="84"/>
-      <c r="L30" s="84"/>
-      <c r="M30" s="84"/>
-      <c r="N30" s="84"/>
-      <c r="O30" s="84"/>
-      <c r="P30" s="86"/>
-      <c r="Q30" s="93"/>
-      <c r="R30" s="82"/>
-      <c r="S30" s="82"/>
-      <c r="T30" s="82"/>
-      <c r="U30" s="91"/>
+      <c r="E30" s="109"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="90"/>
+      <c r="I30" s="90"/>
+      <c r="J30" s="90"/>
+      <c r="K30" s="90"/>
+      <c r="L30" s="90"/>
+      <c r="M30" s="90"/>
+      <c r="N30" s="90"/>
+      <c r="O30" s="90"/>
+      <c r="P30" s="100"/>
+      <c r="Q30" s="107"/>
+      <c r="R30" s="98"/>
+      <c r="S30" s="98"/>
+      <c r="T30" s="98"/>
+      <c r="U30" s="105"/>
       <c r="X30" s="32"/>
       <c r="Y30" s="32"/>
     </row>
@@ -3478,126 +3835,126 @@
       <c r="B31" s="58"/>
       <c r="C31" s="55"/>
       <c r="D31" s="55"/>
-      <c r="E31" s="96"/>
-      <c r="F31" s="85"/>
-      <c r="G31" s="85"/>
-      <c r="H31" s="85"/>
-      <c r="I31" s="85"/>
-      <c r="J31" s="85"/>
-      <c r="K31" s="85"/>
-      <c r="L31" s="85"/>
-      <c r="M31" s="85"/>
-      <c r="N31" s="85"/>
-      <c r="O31" s="85"/>
-      <c r="P31" s="87"/>
-      <c r="Q31" s="94"/>
-      <c r="R31" s="83"/>
-      <c r="S31" s="83"/>
-      <c r="T31" s="83"/>
-      <c r="U31" s="92"/>
+      <c r="E31" s="110"/>
+      <c r="F31" s="91"/>
+      <c r="G31" s="91"/>
+      <c r="H31" s="91"/>
+      <c r="I31" s="91"/>
+      <c r="J31" s="91"/>
+      <c r="K31" s="91"/>
+      <c r="L31" s="91"/>
+      <c r="M31" s="91"/>
+      <c r="N31" s="91"/>
+      <c r="O31" s="91"/>
+      <c r="P31" s="101"/>
+      <c r="Q31" s="108"/>
+      <c r="R31" s="99"/>
+      <c r="S31" s="99"/>
+      <c r="T31" s="99"/>
+      <c r="U31" s="106"/>
       <c r="W31" s="21"/>
       <c r="X31" s="21"/>
       <c r="Y31" s="21"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A32" s="88" t="s">
+      <c r="A32" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="89"/>
-      <c r="C32" s="89"/>
-      <c r="D32" s="89"/>
-      <c r="E32" s="89"/>
-      <c r="F32" s="89"/>
-      <c r="G32" s="89"/>
-      <c r="H32" s="89"/>
-      <c r="I32" s="89"/>
-      <c r="J32" s="89"/>
-      <c r="K32" s="89"/>
-      <c r="L32" s="89"/>
-      <c r="M32" s="89"/>
-      <c r="N32" s="89"/>
-      <c r="O32" s="89"/>
-      <c r="P32" s="89"/>
-      <c r="Q32" s="89"/>
-      <c r="R32" s="89"/>
-      <c r="S32" s="89"/>
-      <c r="T32" s="89"/>
-      <c r="U32" s="90"/>
+      <c r="B32" s="103"/>
+      <c r="C32" s="103"/>
+      <c r="D32" s="103"/>
+      <c r="E32" s="103"/>
+      <c r="F32" s="103"/>
+      <c r="G32" s="103"/>
+      <c r="H32" s="103"/>
+      <c r="I32" s="103"/>
+      <c r="J32" s="103"/>
+      <c r="K32" s="103"/>
+      <c r="L32" s="103"/>
+      <c r="M32" s="103"/>
+      <c r="N32" s="103"/>
+      <c r="O32" s="103"/>
+      <c r="P32" s="103"/>
+      <c r="Q32" s="103"/>
+      <c r="R32" s="103"/>
+      <c r="S32" s="103"/>
+      <c r="T32" s="103"/>
+      <c r="U32" s="104"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A33" s="76" t="s">
+      <c r="A33" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="77"/>
-      <c r="C33" s="77"/>
-      <c r="D33" s="77"/>
-      <c r="E33" s="77"/>
-      <c r="F33" s="77"/>
-      <c r="G33" s="77"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="77"/>
-      <c r="J33" s="77"/>
-      <c r="K33" s="77"/>
-      <c r="L33" s="77"/>
-      <c r="M33" s="77"/>
-      <c r="N33" s="77"/>
-      <c r="O33" s="77"/>
-      <c r="P33" s="77"/>
-      <c r="Q33" s="77"/>
-      <c r="R33" s="77"/>
-      <c r="S33" s="77"/>
-      <c r="T33" s="77"/>
-      <c r="U33" s="78"/>
+      <c r="B33" s="93"/>
+      <c r="C33" s="93"/>
+      <c r="D33" s="93"/>
+      <c r="E33" s="93"/>
+      <c r="F33" s="93"/>
+      <c r="G33" s="93"/>
+      <c r="H33" s="93"/>
+      <c r="I33" s="93"/>
+      <c r="J33" s="93"/>
+      <c r="K33" s="93"/>
+      <c r="L33" s="93"/>
+      <c r="M33" s="93"/>
+      <c r="N33" s="93"/>
+      <c r="O33" s="93"/>
+      <c r="P33" s="93"/>
+      <c r="Q33" s="93"/>
+      <c r="R33" s="93"/>
+      <c r="S33" s="93"/>
+      <c r="T33" s="93"/>
+      <c r="U33" s="94"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A34" s="76" t="s">
+      <c r="A34" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="77"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="77"/>
-      <c r="G34" s="77"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="77"/>
-      <c r="J34" s="77"/>
-      <c r="K34" s="77"/>
-      <c r="L34" s="77"/>
-      <c r="M34" s="77"/>
-      <c r="N34" s="77"/>
-      <c r="O34" s="77"/>
-      <c r="P34" s="77"/>
-      <c r="Q34" s="77"/>
-      <c r="R34" s="77"/>
-      <c r="S34" s="77"/>
-      <c r="T34" s="77"/>
-      <c r="U34" s="78"/>
+      <c r="B34" s="93"/>
+      <c r="C34" s="93"/>
+      <c r="D34" s="93"/>
+      <c r="E34" s="93"/>
+      <c r="F34" s="93"/>
+      <c r="G34" s="93"/>
+      <c r="H34" s="93"/>
+      <c r="I34" s="93"/>
+      <c r="J34" s="93"/>
+      <c r="K34" s="93"/>
+      <c r="L34" s="93"/>
+      <c r="M34" s="93"/>
+      <c r="N34" s="93"/>
+      <c r="O34" s="93"/>
+      <c r="P34" s="93"/>
+      <c r="Q34" s="93"/>
+      <c r="R34" s="93"/>
+      <c r="S34" s="93"/>
+      <c r="T34" s="93"/>
+      <c r="U34" s="94"/>
     </row>
     <row r="35" spans="1:25" s="18" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="79" t="s">
+      <c r="A35" s="95" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="80"/>
-      <c r="C35" s="80"/>
-      <c r="D35" s="80"/>
-      <c r="E35" s="80"/>
-      <c r="F35" s="80"/>
-      <c r="G35" s="80"/>
-      <c r="H35" s="80"/>
-      <c r="I35" s="80"/>
-      <c r="J35" s="80"/>
-      <c r="K35" s="80"/>
-      <c r="L35" s="80"/>
-      <c r="M35" s="80"/>
-      <c r="N35" s="80"/>
-      <c r="O35" s="80"/>
-      <c r="P35" s="80"/>
-      <c r="Q35" s="80"/>
-      <c r="R35" s="80"/>
-      <c r="S35" s="80"/>
-      <c r="T35" s="80"/>
-      <c r="U35" s="81"/>
+      <c r="B35" s="96"/>
+      <c r="C35" s="96"/>
+      <c r="D35" s="96"/>
+      <c r="E35" s="96"/>
+      <c r="F35" s="96"/>
+      <c r="G35" s="96"/>
+      <c r="H35" s="96"/>
+      <c r="I35" s="96"/>
+      <c r="J35" s="96"/>
+      <c r="K35" s="96"/>
+      <c r="L35" s="96"/>
+      <c r="M35" s="96"/>
+      <c r="N35" s="96"/>
+      <c r="O35" s="96"/>
+      <c r="P35" s="96"/>
+      <c r="Q35" s="96"/>
+      <c r="R35" s="96"/>
+      <c r="S35" s="96"/>
+      <c r="T35" s="96"/>
+      <c r="U35" s="97"/>
       <c r="W35" s="21"/>
       <c r="X35" s="22"/>
       <c r="Y35" s="22"/>
@@ -3679,15 +4036,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A3:D4"/>
-    <mergeCell ref="E3:P4"/>
-    <mergeCell ref="E5:P5"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="F26:F31"/>
-    <mergeCell ref="G26:G31"/>
-    <mergeCell ref="N26:N31"/>
-    <mergeCell ref="I26:I31"/>
-    <mergeCell ref="J26:J31"/>
     <mergeCell ref="A34:U34"/>
     <mergeCell ref="A35:U35"/>
     <mergeCell ref="T26:T31"/>
@@ -3704,71 +4052,80 @@
     <mergeCell ref="Q26:Q31"/>
     <mergeCell ref="K26:K31"/>
     <mergeCell ref="E26:E31"/>
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="E3:P4"/>
+    <mergeCell ref="E5:P5"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="F26:F31"/>
+    <mergeCell ref="G26:G31"/>
+    <mergeCell ref="N26:N31"/>
+    <mergeCell ref="I26:I31"/>
+    <mergeCell ref="J26:J31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D38:E38 I38:Y38">
-    <cfRule type="cellIs" dxfId="32" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="26" stopIfTrue="1" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="27" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="27" stopIfTrue="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="28" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="28" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:G6 I6:K6 M6:P6 G7:N7 P7 G8:L8 E9:F9 J9:L9 E10:G10 I10:M10 O10:P10 E11:J11 E12:G12 K12 E13:H13 J13:N13 P13 N14:P14 E14:I15 M15:O15 E16:J16 L16:P16 E17:I17 K17:P17 E18:P25">
-    <cfRule type="cellIs" dxfId="29" priority="29" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="29" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="30" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="30" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="31" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="31" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="26" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="13" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="14" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="15" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="23" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="10" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="11" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="12" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11:P12">
-    <cfRule type="cellIs" dxfId="20" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="1" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="2" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8:P9">
-    <cfRule type="cellIs" dxfId="17" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="16" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="17" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="18" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3785,8 +4142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52089AA5-E353-4911-A982-D49FBFB6A530}">
   <dimension ref="A1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U38" sqref="A2:U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3839,26 +4196,26 @@
       <c r="Y2" s="14"/>
     </row>
     <row r="3" spans="1:25" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="98"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="101" t="s">
+      <c r="B3" s="80"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="101"/>
-      <c r="G3" s="101"/>
-      <c r="H3" s="101"/>
-      <c r="I3" s="101"/>
-      <c r="J3" s="101"/>
-      <c r="K3" s="101"/>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="N3" s="101"/>
-      <c r="O3" s="101"/>
-      <c r="P3" s="101"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
+      <c r="H3" s="83"/>
+      <c r="I3" s="83"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="83"/>
+      <c r="M3" s="83"/>
+      <c r="N3" s="83"/>
+      <c r="O3" s="83"/>
+      <c r="P3" s="83"/>
       <c r="Q3" s="66"/>
       <c r="R3" s="66"/>
       <c r="S3" s="66"/>
@@ -3869,22 +4226,22 @@
       <c r="Y3" s="14"/>
     </row>
     <row r="4" spans="1:25" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="99"/>
-      <c r="B4" s="100"/>
-      <c r="C4" s="100"/>
-      <c r="D4" s="100"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="102"/>
-      <c r="L4" s="102"/>
-      <c r="M4" s="102"/>
-      <c r="N4" s="102"/>
-      <c r="O4" s="102"/>
-      <c r="P4" s="102"/>
+      <c r="A4" s="81"/>
+      <c r="B4" s="82"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="84"/>
+      <c r="L4" s="84"/>
+      <c r="M4" s="84"/>
+      <c r="N4" s="84"/>
+      <c r="O4" s="84"/>
+      <c r="P4" s="84"/>
       <c r="Q4" s="68"/>
       <c r="R4" s="68"/>
       <c r="S4" s="68"/>
@@ -3901,27 +4258,27 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="103" t="s">
+      <c r="E5" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="104"/>
-      <c r="G5" s="104"/>
-      <c r="H5" s="104"/>
-      <c r="I5" s="104"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
-      <c r="M5" s="104"/>
-      <c r="N5" s="105"/>
-      <c r="O5" s="105"/>
-      <c r="P5" s="106"/>
-      <c r="Q5" s="107" t="s">
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="86"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="88"/>
+      <c r="Q5" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="R5" s="104"/>
-      <c r="S5" s="104"/>
-      <c r="T5" s="104"/>
-      <c r="U5" s="106"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="86"/>
+      <c r="T5" s="86"/>
+      <c r="U5" s="88"/>
       <c r="W5" s="21"/>
       <c r="X5" s="22"/>
       <c r="Y5" s="22"/>
@@ -4099,7 +4456,7 @@
       <c r="B10" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="111"/>
+      <c r="D10" s="78"/>
       <c r="M10" s="37" t="s">
         <v>5</v>
       </c>
@@ -4109,8 +4466,8 @@
       <c r="O10" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="P10" s="111"/>
-      <c r="U10" s="111"/>
+      <c r="P10" s="78"/>
+      <c r="U10" s="78"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
@@ -4119,7 +4476,7 @@
       <c r="B11" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="111"/>
+      <c r="D11" s="78"/>
       <c r="M11" s="37" t="s">
         <v>5</v>
       </c>
@@ -4129,8 +4486,8 @@
       <c r="O11" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="P11" s="111"/>
-      <c r="U11" s="111"/>
+      <c r="P11" s="78"/>
+      <c r="U11" s="78"/>
     </row>
     <row r="12" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="33">
@@ -4436,10 +4793,10 @@
       <c r="O19" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="P19" s="108" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q19" s="109" t="s">
+      <c r="P19" s="76" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="77" t="s">
         <v>4</v>
       </c>
       <c r="R19" s="73" t="s">
@@ -4462,9 +4819,9 @@
       <c r="A20" s="2">
         <v>12</v>
       </c>
-      <c r="D20" s="111"/>
-      <c r="P20" s="111"/>
-      <c r="U20" s="111"/>
+      <c r="D20" s="78"/>
+      <c r="P20" s="78"/>
+      <c r="U20" s="78"/>
     </row>
     <row r="21" spans="1:25" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="33">
@@ -4611,55 +4968,55 @@
       <c r="B26" s="54"/>
       <c r="C26" s="55"/>
       <c r="D26" s="55"/>
-      <c r="E26" s="95" t="s">
+      <c r="E26" s="109" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="84" t="s">
+      <c r="F26" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="84" t="s">
+      <c r="G26" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="H26" s="84" t="s">
+      <c r="H26" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="I26" s="84" t="s">
+      <c r="I26" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="J26" s="84" t="s">
+      <c r="J26" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="K26" s="84" t="s">
+      <c r="K26" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="L26" s="84" t="s">
+      <c r="L26" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="M26" s="84" t="s">
+      <c r="M26" s="90" t="s">
         <v>15</v>
       </c>
-      <c r="N26" s="84" t="s">
+      <c r="N26" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="O26" s="84" t="s">
+      <c r="O26" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="P26" s="86" t="s">
+      <c r="P26" s="100" t="s">
         <v>18</v>
       </c>
-      <c r="Q26" s="93" t="s">
+      <c r="Q26" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="R26" s="82" t="s">
+      <c r="R26" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="S26" s="82" t="s">
+      <c r="S26" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="T26" s="82" t="s">
+      <c r="T26" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="U26" s="91" t="s">
+      <c r="U26" s="105" t="s">
         <v>31</v>
       </c>
       <c r="W26" s="31"/>
@@ -4671,23 +5028,23 @@
       <c r="B27" s="56"/>
       <c r="C27" s="55"/>
       <c r="D27" s="55"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="84"/>
-      <c r="G27" s="84"/>
-      <c r="H27" s="84"/>
-      <c r="I27" s="84"/>
-      <c r="J27" s="84"/>
-      <c r="K27" s="84"/>
-      <c r="L27" s="84"/>
-      <c r="M27" s="84"/>
-      <c r="N27" s="84"/>
-      <c r="O27" s="84"/>
-      <c r="P27" s="86"/>
-      <c r="Q27" s="93"/>
-      <c r="R27" s="82"/>
-      <c r="S27" s="82"/>
-      <c r="T27" s="82"/>
-      <c r="U27" s="91"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="90"/>
+      <c r="J27" s="90"/>
+      <c r="K27" s="90"/>
+      <c r="L27" s="90"/>
+      <c r="M27" s="90"/>
+      <c r="N27" s="90"/>
+      <c r="O27" s="90"/>
+      <c r="P27" s="100"/>
+      <c r="Q27" s="107"/>
+      <c r="R27" s="98"/>
+      <c r="S27" s="98"/>
+      <c r="T27" s="98"/>
+      <c r="U27" s="105"/>
       <c r="W27" s="31"/>
       <c r="X27" s="32"/>
       <c r="Y27" s="32"/>
@@ -4697,23 +5054,23 @@
       <c r="B28" s="56"/>
       <c r="C28" s="55"/>
       <c r="D28" s="55"/>
-      <c r="E28" s="95"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="84"/>
-      <c r="I28" s="84"/>
-      <c r="J28" s="84"/>
-      <c r="K28" s="84"/>
-      <c r="L28" s="84"/>
-      <c r="M28" s="84"/>
-      <c r="N28" s="84"/>
-      <c r="O28" s="84"/>
-      <c r="P28" s="86"/>
-      <c r="Q28" s="93"/>
-      <c r="R28" s="82"/>
-      <c r="S28" s="82"/>
-      <c r="T28" s="82"/>
-      <c r="U28" s="91"/>
+      <c r="E28" s="109"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="90"/>
+      <c r="H28" s="90"/>
+      <c r="I28" s="90"/>
+      <c r="J28" s="90"/>
+      <c r="K28" s="90"/>
+      <c r="L28" s="90"/>
+      <c r="M28" s="90"/>
+      <c r="N28" s="90"/>
+      <c r="O28" s="90"/>
+      <c r="P28" s="100"/>
+      <c r="Q28" s="107"/>
+      <c r="R28" s="98"/>
+      <c r="S28" s="98"/>
+      <c r="T28" s="98"/>
+      <c r="U28" s="105"/>
       <c r="W28" s="31"/>
       <c r="X28" s="32"/>
       <c r="Y28" s="32"/>
@@ -4723,23 +5080,23 @@
       <c r="B29" s="57"/>
       <c r="C29" s="55"/>
       <c r="D29" s="55"/>
-      <c r="E29" s="95"/>
-      <c r="F29" s="84"/>
-      <c r="G29" s="84"/>
-      <c r="H29" s="84"/>
-      <c r="I29" s="84"/>
-      <c r="J29" s="84"/>
-      <c r="K29" s="84"/>
-      <c r="L29" s="84"/>
-      <c r="M29" s="84"/>
-      <c r="N29" s="84"/>
-      <c r="O29" s="84"/>
-      <c r="P29" s="86"/>
-      <c r="Q29" s="93"/>
-      <c r="R29" s="82"/>
-      <c r="S29" s="82"/>
-      <c r="T29" s="82"/>
-      <c r="U29" s="91"/>
+      <c r="E29" s="109"/>
+      <c r="F29" s="90"/>
+      <c r="G29" s="90"/>
+      <c r="H29" s="90"/>
+      <c r="I29" s="90"/>
+      <c r="J29" s="90"/>
+      <c r="K29" s="90"/>
+      <c r="L29" s="90"/>
+      <c r="M29" s="90"/>
+      <c r="N29" s="90"/>
+      <c r="O29" s="90"/>
+      <c r="P29" s="100"/>
+      <c r="Q29" s="107"/>
+      <c r="R29" s="98"/>
+      <c r="S29" s="98"/>
+      <c r="T29" s="98"/>
+      <c r="U29" s="105"/>
       <c r="X29" s="32"/>
       <c r="Y29" s="32"/>
     </row>
@@ -4748,23 +5105,23 @@
       <c r="B30" s="54"/>
       <c r="C30" s="55"/>
       <c r="D30" s="55"/>
-      <c r="E30" s="95"/>
-      <c r="F30" s="84"/>
-      <c r="G30" s="84"/>
-      <c r="H30" s="84"/>
-      <c r="I30" s="84"/>
-      <c r="J30" s="84"/>
-      <c r="K30" s="84"/>
-      <c r="L30" s="84"/>
-      <c r="M30" s="84"/>
-      <c r="N30" s="84"/>
-      <c r="O30" s="84"/>
-      <c r="P30" s="86"/>
-      <c r="Q30" s="93"/>
-      <c r="R30" s="82"/>
-      <c r="S30" s="82"/>
-      <c r="T30" s="82"/>
-      <c r="U30" s="91"/>
+      <c r="E30" s="109"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="90"/>
+      <c r="I30" s="90"/>
+      <c r="J30" s="90"/>
+      <c r="K30" s="90"/>
+      <c r="L30" s="90"/>
+      <c r="M30" s="90"/>
+      <c r="N30" s="90"/>
+      <c r="O30" s="90"/>
+      <c r="P30" s="100"/>
+      <c r="Q30" s="107"/>
+      <c r="R30" s="98"/>
+      <c r="S30" s="98"/>
+      <c r="T30" s="98"/>
+      <c r="U30" s="105"/>
       <c r="X30" s="32"/>
       <c r="Y30" s="32"/>
     </row>
@@ -4773,126 +5130,126 @@
       <c r="B31" s="58"/>
       <c r="C31" s="55"/>
       <c r="D31" s="55"/>
-      <c r="E31" s="96"/>
-      <c r="F31" s="85"/>
-      <c r="G31" s="85"/>
-      <c r="H31" s="85"/>
-      <c r="I31" s="85"/>
-      <c r="J31" s="85"/>
-      <c r="K31" s="85"/>
-      <c r="L31" s="85"/>
-      <c r="M31" s="85"/>
-      <c r="N31" s="85"/>
-      <c r="O31" s="85"/>
-      <c r="P31" s="87"/>
-      <c r="Q31" s="94"/>
-      <c r="R31" s="83"/>
-      <c r="S31" s="83"/>
-      <c r="T31" s="83"/>
-      <c r="U31" s="92"/>
+      <c r="E31" s="110"/>
+      <c r="F31" s="91"/>
+      <c r="G31" s="91"/>
+      <c r="H31" s="91"/>
+      <c r="I31" s="91"/>
+      <c r="J31" s="91"/>
+      <c r="K31" s="91"/>
+      <c r="L31" s="91"/>
+      <c r="M31" s="91"/>
+      <c r="N31" s="91"/>
+      <c r="O31" s="91"/>
+      <c r="P31" s="101"/>
+      <c r="Q31" s="108"/>
+      <c r="R31" s="99"/>
+      <c r="S31" s="99"/>
+      <c r="T31" s="99"/>
+      <c r="U31" s="106"/>
       <c r="W31" s="21"/>
       <c r="X31" s="21"/>
       <c r="Y31" s="21"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A32" s="110" t="s">
+      <c r="A32" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="89"/>
-      <c r="C32" s="89"/>
-      <c r="D32" s="89"/>
-      <c r="E32" s="89"/>
-      <c r="F32" s="89"/>
-      <c r="G32" s="89"/>
-      <c r="H32" s="89"/>
-      <c r="I32" s="89"/>
-      <c r="J32" s="89"/>
-      <c r="K32" s="89"/>
-      <c r="L32" s="89"/>
-      <c r="M32" s="89"/>
-      <c r="N32" s="89"/>
-      <c r="O32" s="89"/>
-      <c r="P32" s="89"/>
-      <c r="Q32" s="89"/>
-      <c r="R32" s="89"/>
-      <c r="S32" s="89"/>
-      <c r="T32" s="89"/>
-      <c r="U32" s="90"/>
+      <c r="B32" s="103"/>
+      <c r="C32" s="103"/>
+      <c r="D32" s="103"/>
+      <c r="E32" s="103"/>
+      <c r="F32" s="103"/>
+      <c r="G32" s="103"/>
+      <c r="H32" s="103"/>
+      <c r="I32" s="103"/>
+      <c r="J32" s="103"/>
+      <c r="K32" s="103"/>
+      <c r="L32" s="103"/>
+      <c r="M32" s="103"/>
+      <c r="N32" s="103"/>
+      <c r="O32" s="103"/>
+      <c r="P32" s="103"/>
+      <c r="Q32" s="103"/>
+      <c r="R32" s="103"/>
+      <c r="S32" s="103"/>
+      <c r="T32" s="103"/>
+      <c r="U32" s="104"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A33" s="112" t="s">
+      <c r="A33" s="111" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="77"/>
-      <c r="C33" s="77"/>
-      <c r="D33" s="77"/>
-      <c r="E33" s="77"/>
-      <c r="F33" s="77"/>
-      <c r="G33" s="77"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="77"/>
-      <c r="J33" s="77"/>
-      <c r="K33" s="77"/>
-      <c r="L33" s="77"/>
-      <c r="M33" s="77"/>
-      <c r="N33" s="77"/>
-      <c r="O33" s="77"/>
-      <c r="P33" s="77"/>
-      <c r="Q33" s="77"/>
-      <c r="R33" s="77"/>
-      <c r="S33" s="77"/>
-      <c r="T33" s="77"/>
-      <c r="U33" s="78"/>
+      <c r="B33" s="93"/>
+      <c r="C33" s="93"/>
+      <c r="D33" s="93"/>
+      <c r="E33" s="93"/>
+      <c r="F33" s="93"/>
+      <c r="G33" s="93"/>
+      <c r="H33" s="93"/>
+      <c r="I33" s="93"/>
+      <c r="J33" s="93"/>
+      <c r="K33" s="93"/>
+      <c r="L33" s="93"/>
+      <c r="M33" s="93"/>
+      <c r="N33" s="93"/>
+      <c r="O33" s="93"/>
+      <c r="P33" s="93"/>
+      <c r="Q33" s="93"/>
+      <c r="R33" s="93"/>
+      <c r="S33" s="93"/>
+      <c r="T33" s="93"/>
+      <c r="U33" s="94"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A34" s="112" t="s">
+      <c r="A34" s="111" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="77"/>
-      <c r="C34" s="77"/>
-      <c r="D34" s="77"/>
-      <c r="E34" s="77"/>
-      <c r="F34" s="77"/>
-      <c r="G34" s="77"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="77"/>
-      <c r="J34" s="77"/>
-      <c r="K34" s="77"/>
-      <c r="L34" s="77"/>
-      <c r="M34" s="77"/>
-      <c r="N34" s="77"/>
-      <c r="O34" s="77"/>
-      <c r="P34" s="77"/>
-      <c r="Q34" s="77"/>
-      <c r="R34" s="77"/>
-      <c r="S34" s="77"/>
-      <c r="T34" s="77"/>
-      <c r="U34" s="78"/>
+      <c r="B34" s="93"/>
+      <c r="C34" s="93"/>
+      <c r="D34" s="93"/>
+      <c r="E34" s="93"/>
+      <c r="F34" s="93"/>
+      <c r="G34" s="93"/>
+      <c r="H34" s="93"/>
+      <c r="I34" s="93"/>
+      <c r="J34" s="93"/>
+      <c r="K34" s="93"/>
+      <c r="L34" s="93"/>
+      <c r="M34" s="93"/>
+      <c r="N34" s="93"/>
+      <c r="O34" s="93"/>
+      <c r="P34" s="93"/>
+      <c r="Q34" s="93"/>
+      <c r="R34" s="93"/>
+      <c r="S34" s="93"/>
+      <c r="T34" s="93"/>
+      <c r="U34" s="94"/>
     </row>
     <row r="35" spans="1:25" s="18" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="79" t="s">
+      <c r="A35" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="80"/>
-      <c r="C35" s="80"/>
-      <c r="D35" s="80"/>
-      <c r="E35" s="80"/>
-      <c r="F35" s="80"/>
-      <c r="G35" s="80"/>
-      <c r="H35" s="80"/>
-      <c r="I35" s="80"/>
-      <c r="J35" s="80"/>
-      <c r="K35" s="80"/>
-      <c r="L35" s="80"/>
-      <c r="M35" s="80"/>
-      <c r="N35" s="80"/>
-      <c r="O35" s="80"/>
-      <c r="P35" s="80"/>
-      <c r="Q35" s="80"/>
-      <c r="R35" s="80"/>
-      <c r="S35" s="80"/>
-      <c r="T35" s="80"/>
-      <c r="U35" s="81"/>
+      <c r="B35" s="96"/>
+      <c r="C35" s="96"/>
+      <c r="D35" s="96"/>
+      <c r="E35" s="96"/>
+      <c r="F35" s="96"/>
+      <c r="G35" s="96"/>
+      <c r="H35" s="96"/>
+      <c r="I35" s="96"/>
+      <c r="J35" s="96"/>
+      <c r="K35" s="96"/>
+      <c r="L35" s="96"/>
+      <c r="M35" s="96"/>
+      <c r="N35" s="96"/>
+      <c r="O35" s="96"/>
+      <c r="P35" s="96"/>
+      <c r="Q35" s="96"/>
+      <c r="R35" s="96"/>
+      <c r="S35" s="96"/>
+      <c r="T35" s="96"/>
+      <c r="U35" s="97"/>
       <c r="W35" s="21"/>
       <c r="X35" s="22"/>
       <c r="Y35" s="22"/>
@@ -4974,6 +5331,16 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="E3:P4"/>
+    <mergeCell ref="E5:P5"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="E26:E31"/>
+    <mergeCell ref="F26:F31"/>
+    <mergeCell ref="G26:G31"/>
+    <mergeCell ref="H26:H31"/>
+    <mergeCell ref="I26:I31"/>
+    <mergeCell ref="J26:J31"/>
     <mergeCell ref="A33:U33"/>
     <mergeCell ref="A34:U34"/>
     <mergeCell ref="A35:U35"/>
@@ -4989,69 +5356,59 @@
     <mergeCell ref="N26:N31"/>
     <mergeCell ref="O26:O31"/>
     <mergeCell ref="P26:P31"/>
-    <mergeCell ref="A3:D4"/>
-    <mergeCell ref="E3:P4"/>
-    <mergeCell ref="E5:P5"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="E26:E31"/>
-    <mergeCell ref="F26:F31"/>
-    <mergeCell ref="G26:G31"/>
-    <mergeCell ref="H26:H31"/>
-    <mergeCell ref="I26:I31"/>
-    <mergeCell ref="J26:J31"/>
   </mergeCells>
   <conditionalFormatting sqref="D38:E38 I38:Y38">
-    <cfRule type="cellIs" dxfId="14" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="13" stopIfTrue="1" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="15" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F6:G6 I6:K6 M6:P6 P7 G7:L8 E9:F9 J9:L9 I13:L13 E14:J14 E12:G13 K12 E15:H15 J15:N15 P15 N16:P16 E16:I17 M17:O17 E18:J18 L18:P18 E19:I19 K19:L19 E21:P25 M14:P14 O13:P13 P12">
-    <cfRule type="cellIs" dxfId="11" priority="16" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="F6:G6 I6:K6 M6:P6 P7 G7:L8 E9:F9 J9:L9 K12 P12 E12:G13 I13:L13 O13:P13 E14:J14 M14:P14 E15:H15 J15:N15 P15 N16:P16 E16:I17 M17:O17 E18:J18 L18:P18 E19:I19 K19:L19 E21:P25">
+    <cfRule type="cellIs" dxfId="26" priority="16" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="17" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="18" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="8" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="7" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="8" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="9" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="5" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="4" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="5" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8:P8 P9">
-    <cfRule type="cellIs" dxfId="2" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="11" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="12" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5059,4 +5416,1261 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50661F68-A50F-4C74-B3DE-EB252B9D0F85}">
+  <dimension ref="A1:U37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="79" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="83" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="83"/>
+      <c r="N2" s="83"/>
+      <c r="O2" s="83"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="67"/>
+    </row>
+    <row r="3" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="81"/>
+      <c r="B3" s="82"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="84"/>
+      <c r="M3" s="84"/>
+      <c r="N3" s="84"/>
+      <c r="O3" s="84"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="69"/>
+    </row>
+    <row r="4" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="85" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="86"/>
+      <c r="N4" s="87"/>
+      <c r="O4" s="87"/>
+      <c r="P4" s="88"/>
+      <c r="Q4" s="89" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" s="86"/>
+      <c r="S4" s="86"/>
+      <c r="T4" s="86"/>
+      <c r="U4" s="88"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" s="24">
+        <v>1</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="70"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S5" s="29"/>
+      <c r="T5" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U5" s="30"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" s="33">
+        <v>2</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="N6" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S6" s="40"/>
+      <c r="T6" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U6" s="41"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" s="33">
+        <v>3</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="41"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" s="33">
+        <v>4</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="37"/>
+      <c r="I8" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="N8" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="O8" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="40"/>
+      <c r="S8" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="T8" s="40"/>
+      <c r="U8" s="41"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="N9" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="O9" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9" s="78"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="78"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="O10" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P10" s="78"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="78"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11" s="33">
+        <v>4.3</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="37"/>
+      <c r="J11" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="37"/>
+      <c r="L11" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="M11" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="O11" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="40"/>
+      <c r="S11" s="40"/>
+      <c r="T11" s="40"/>
+      <c r="U11" s="41"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" s="33">
+        <v>5</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="N12" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="O12" s="37"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="40"/>
+      <c r="T12" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U12" s="41"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" s="33">
+        <v>6</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="L13" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="R13" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S13" s="40"/>
+      <c r="T13" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U13" s="41"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" s="33">
+        <v>7</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="R14" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S14" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="T14" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U14" s="75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" s="33">
+        <v>8</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="K15" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="L15" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="M15" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" s="33">
+        <v>9</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="37"/>
+      <c r="P16" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="40"/>
+      <c r="S16" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="T16" s="40"/>
+      <c r="U16" s="41"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" s="33">
+        <v>10</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="40"/>
+      <c r="U17" s="75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18" s="33">
+        <v>11</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="N18" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="O18" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P18" s="76" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="R18" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S18" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="T18" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U18" s="75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="O19" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P19" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="T19" s="1"/>
+      <c r="U19" s="78"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A20" s="33">
+        <v>13</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="O20" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P20" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="R20" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S20" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="T20" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U20" s="73" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" s="33">
+        <v>14</v>
+      </c>
+      <c r="B21" s="42"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="41"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A22" s="33">
+        <v>15</v>
+      </c>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="39"/>
+      <c r="R22" s="40"/>
+      <c r="S22" s="40"/>
+      <c r="T22" s="40"/>
+      <c r="U22" s="41"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A23" s="33">
+        <v>16</v>
+      </c>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="37"/>
+      <c r="O23" s="37"/>
+      <c r="P23" s="38"/>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="40"/>
+      <c r="S23" s="40"/>
+      <c r="T23" s="40"/>
+      <c r="U23" s="41"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A24" s="44">
+        <v>17</v>
+      </c>
+      <c r="B24" s="45"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="48"/>
+      <c r="O24" s="48"/>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="50"/>
+      <c r="R24" s="51"/>
+      <c r="S24" s="51"/>
+      <c r="T24" s="51"/>
+      <c r="U24" s="52"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A25" s="53"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="109" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="90" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="90" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="90" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="90" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="90" t="s">
+        <v>13</v>
+      </c>
+      <c r="L25" s="90" t="s">
+        <v>14</v>
+      </c>
+      <c r="M25" s="90" t="s">
+        <v>15</v>
+      </c>
+      <c r="N25" s="90" t="s">
+        <v>16</v>
+      </c>
+      <c r="O25" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="P25" s="100" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q25" s="107" t="s">
+        <v>19</v>
+      </c>
+      <c r="R25" s="98" t="s">
+        <v>20</v>
+      </c>
+      <c r="S25" s="98" t="s">
+        <v>21</v>
+      </c>
+      <c r="T25" s="98" t="s">
+        <v>30</v>
+      </c>
+      <c r="U25" s="105" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="53"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="109"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="90"/>
+      <c r="H26" s="90"/>
+      <c r="I26" s="90"/>
+      <c r="J26" s="90"/>
+      <c r="K26" s="90"/>
+      <c r="L26" s="90"/>
+      <c r="M26" s="90"/>
+      <c r="N26" s="90"/>
+      <c r="O26" s="90"/>
+      <c r="P26" s="100"/>
+      <c r="Q26" s="107"/>
+      <c r="R26" s="98"/>
+      <c r="S26" s="98"/>
+      <c r="T26" s="98"/>
+      <c r="U26" s="105"/>
+    </row>
+    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="53"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="90"/>
+      <c r="G27" s="90"/>
+      <c r="H27" s="90"/>
+      <c r="I27" s="90"/>
+      <c r="J27" s="90"/>
+      <c r="K27" s="90"/>
+      <c r="L27" s="90"/>
+      <c r="M27" s="90"/>
+      <c r="N27" s="90"/>
+      <c r="O27" s="90"/>
+      <c r="P27" s="100"/>
+      <c r="Q27" s="107"/>
+      <c r="R27" s="98"/>
+      <c r="S27" s="98"/>
+      <c r="T27" s="98"/>
+      <c r="U27" s="105"/>
+    </row>
+    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="53"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="109"/>
+      <c r="F28" s="90"/>
+      <c r="G28" s="90"/>
+      <c r="H28" s="90"/>
+      <c r="I28" s="90"/>
+      <c r="J28" s="90"/>
+      <c r="K28" s="90"/>
+      <c r="L28" s="90"/>
+      <c r="M28" s="90"/>
+      <c r="N28" s="90"/>
+      <c r="O28" s="90"/>
+      <c r="P28" s="100"/>
+      <c r="Q28" s="107"/>
+      <c r="R28" s="98"/>
+      <c r="S28" s="98"/>
+      <c r="T28" s="98"/>
+      <c r="U28" s="105"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A29" s="53"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="109"/>
+      <c r="F29" s="90"/>
+      <c r="G29" s="90"/>
+      <c r="H29" s="90"/>
+      <c r="I29" s="90"/>
+      <c r="J29" s="90"/>
+      <c r="K29" s="90"/>
+      <c r="L29" s="90"/>
+      <c r="M29" s="90"/>
+      <c r="N29" s="90"/>
+      <c r="O29" s="90"/>
+      <c r="P29" s="100"/>
+      <c r="Q29" s="107"/>
+      <c r="R29" s="98"/>
+      <c r="S29" s="98"/>
+      <c r="T29" s="98"/>
+      <c r="U29" s="105"/>
+    </row>
+    <row r="30" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="53"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="110"/>
+      <c r="F30" s="91"/>
+      <c r="G30" s="91"/>
+      <c r="H30" s="91"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="91"/>
+      <c r="K30" s="91"/>
+      <c r="L30" s="91"/>
+      <c r="M30" s="91"/>
+      <c r="N30" s="91"/>
+      <c r="O30" s="91"/>
+      <c r="P30" s="101"/>
+      <c r="Q30" s="108"/>
+      <c r="R30" s="99"/>
+      <c r="S30" s="99"/>
+      <c r="T30" s="99"/>
+      <c r="U30" s="106"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A31" s="112" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="103"/>
+      <c r="C31" s="103"/>
+      <c r="D31" s="103"/>
+      <c r="E31" s="103"/>
+      <c r="F31" s="103"/>
+      <c r="G31" s="103"/>
+      <c r="H31" s="103"/>
+      <c r="I31" s="103"/>
+      <c r="J31" s="103"/>
+      <c r="K31" s="103"/>
+      <c r="L31" s="103"/>
+      <c r="M31" s="103"/>
+      <c r="N31" s="103"/>
+      <c r="O31" s="103"/>
+      <c r="P31" s="103"/>
+      <c r="Q31" s="103"/>
+      <c r="R31" s="103"/>
+      <c r="S31" s="103"/>
+      <c r="T31" s="103"/>
+      <c r="U31" s="104"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A32" s="111" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="93"/>
+      <c r="C32" s="93"/>
+      <c r="D32" s="93"/>
+      <c r="E32" s="93"/>
+      <c r="F32" s="93"/>
+      <c r="G32" s="93"/>
+      <c r="H32" s="93"/>
+      <c r="I32" s="93"/>
+      <c r="J32" s="93"/>
+      <c r="K32" s="93"/>
+      <c r="L32" s="93"/>
+      <c r="M32" s="93"/>
+      <c r="N32" s="93"/>
+      <c r="O32" s="93"/>
+      <c r="P32" s="93"/>
+      <c r="Q32" s="93"/>
+      <c r="R32" s="93"/>
+      <c r="S32" s="93"/>
+      <c r="T32" s="93"/>
+      <c r="U32" s="94"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A33" s="111" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="93"/>
+      <c r="C33" s="93"/>
+      <c r="D33" s="93"/>
+      <c r="E33" s="93"/>
+      <c r="F33" s="93"/>
+      <c r="G33" s="93"/>
+      <c r="H33" s="93"/>
+      <c r="I33" s="93"/>
+      <c r="J33" s="93"/>
+      <c r="K33" s="93"/>
+      <c r="L33" s="93"/>
+      <c r="M33" s="93"/>
+      <c r="N33" s="93"/>
+      <c r="O33" s="93"/>
+      <c r="P33" s="93"/>
+      <c r="Q33" s="93"/>
+      <c r="R33" s="93"/>
+      <c r="S33" s="93"/>
+      <c r="T33" s="93"/>
+      <c r="U33" s="94"/>
+    </row>
+    <row r="34" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="95"/>
+      <c r="B34" s="96"/>
+      <c r="C34" s="96"/>
+      <c r="D34" s="96"/>
+      <c r="E34" s="96"/>
+      <c r="F34" s="96"/>
+      <c r="G34" s="96"/>
+      <c r="H34" s="96"/>
+      <c r="I34" s="96"/>
+      <c r="J34" s="96"/>
+      <c r="K34" s="96"/>
+      <c r="L34" s="96"/>
+      <c r="M34" s="96"/>
+      <c r="N34" s="96"/>
+      <c r="O34" s="96"/>
+      <c r="P34" s="96"/>
+      <c r="Q34" s="96"/>
+      <c r="R34" s="96"/>
+      <c r="S34" s="96"/>
+      <c r="T34" s="96"/>
+      <c r="U34" s="97"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="18"/>
+      <c r="U35" s="18"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" s="59">
+        <v>152</v>
+      </c>
+      <c r="H36" s="63">
+        <v>153</v>
+      </c>
+      <c r="I36" s="64"/>
+      <c r="J36" s="64"/>
+      <c r="K36" s="60"/>
+      <c r="L36" s="60"/>
+      <c r="M36" s="60"/>
+      <c r="N36" s="60"/>
+      <c r="O36" s="60"/>
+      <c r="P36" s="60"/>
+      <c r="Q36" s="60"/>
+      <c r="R36" s="60"/>
+      <c r="S36" s="60"/>
+      <c r="T36" s="60"/>
+      <c r="U36" s="60"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="H37" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="I37" s="61"/>
+      <c r="J37" s="61"/>
+      <c r="K37" s="61"/>
+      <c r="L37" s="61"/>
+      <c r="M37" s="61"/>
+      <c r="N37" s="61"/>
+      <c r="O37" s="61"/>
+      <c r="P37" s="61"/>
+      <c r="Q37" s="61"/>
+      <c r="R37" s="61"/>
+      <c r="S37" s="61"/>
+      <c r="T37" s="61"/>
+      <c r="U37" s="61"/>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="A32:U32"/>
+    <mergeCell ref="A33:U33"/>
+    <mergeCell ref="A34:U34"/>
+    <mergeCell ref="Q25:Q30"/>
+    <mergeCell ref="R25:R30"/>
+    <mergeCell ref="S25:S30"/>
+    <mergeCell ref="T25:T30"/>
+    <mergeCell ref="U25:U30"/>
+    <mergeCell ref="A31:U31"/>
+    <mergeCell ref="K25:K30"/>
+    <mergeCell ref="L25:L30"/>
+    <mergeCell ref="M25:M30"/>
+    <mergeCell ref="N25:N30"/>
+    <mergeCell ref="O25:O30"/>
+    <mergeCell ref="P25:P30"/>
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="E2:P3"/>
+    <mergeCell ref="E4:P4"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="E25:E30"/>
+    <mergeCell ref="F25:F30"/>
+    <mergeCell ref="G25:G30"/>
+    <mergeCell ref="H25:H30"/>
+    <mergeCell ref="I25:I30"/>
+    <mergeCell ref="J25:J30"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D37:E37 I37:U37">
+    <cfRule type="cellIs" dxfId="14" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"G"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:G5 I5:K5 M5:P5 P6 G6:L7 E8:F8 J8:L8 K11 P11 E11:G12 I12:L12 O12:P12 E13:J13 M13:P13 E14:H14 J14:N14 P14 N15:P15 E15:I16 M16:O16 E17:J17 L17:P17 E18:I18 K18:L18 E21:P24 E20:M20">
+    <cfRule type="cellIs" dxfId="11" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="cellIs" dxfId="8" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="5" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N7:P7 P8">
+    <cfRule type="cellIs" dxfId="2" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
API for like button works again. Will fix the API for the dislike button tomorrow.
</commit_message>
<xml_diff>
--- a/data/docs/Project Manager Report Book.xlsx
+++ b/data/docs/Project Manager Report Book.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files\Ampps\www\video-player\data\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Debian\home\smocloud\Ampps\www\video-player\data\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945FEBAE-FAC6-4BAB-8657-7EC76B094158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DB2F61-F409-41D3-AC3E-72D56E83A9F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11235" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11235" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feb 2025 01-15" sheetId="45818" r:id="rId1"/>
     <sheet name="Feb 2025 16-28" sheetId="45819" r:id="rId2"/>
     <sheet name="Mar 2025 01-21" sheetId="45820" r:id="rId3"/>
+    <sheet name="Mar-Apr 2025 22-04" sheetId="45821" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Feb 2025 01-15'!$A$2:$U$35</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="63">
   <si>
     <t>Major Tasks</t>
   </si>
@@ -248,6 +249,18 @@
   <si>
     <t>I'm not a good project manager. I'm not good at anything.</t>
   </si>
+  <si>
+    <t>Hunter is still tweaking the UI/UX of the video player with Ashton's help.</t>
+  </si>
+  <si>
+    <t>Zach has been working on the poster.</t>
+  </si>
+  <si>
+    <t>Still working on the API, merged it into main (Mikel).</t>
+  </si>
+  <si>
+    <t>Logan will be helping me with the API implementation and writing fetch requests.</t>
+  </si>
 </sst>
 </file>
 
@@ -353,7 +366,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="53">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -1029,13 +1042,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="hair">
+        <color indexed="22"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -1294,38 +1322,37 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="17" fontId="5" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
@@ -1335,38 +1362,6 @@
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="2" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="17" fontId="5" fillId="0" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
       <protection locked="0"/>
@@ -1411,12 +1406,49 @@
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="53" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1425,7 +1457,151 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Project Matrix" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="63">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="10"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="42"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="43"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="10"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="42"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="43"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="10"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="42"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="43"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="10"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="42"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="43"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="10"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="43"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="mediumGray">
+          <fgColor indexed="42"/>
+          <bgColor indexed="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -2492,6 +2668,203 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Text Box 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1467CBB3-E0EA-4654-8EFC-1FE4AE9C5FAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1371600" y="4086225"/>
+          <a:ext cx="685800" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>Major Tasks</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Text Box 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E81D0AF-B87E-4868-AC45-BAA00FE0F49A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1085850" y="4962525"/>
+          <a:ext cx="1000125" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="27432" rIns="36576" bIns="0" anchor="t" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>Summary &amp; Forecast</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1276350</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Text Box 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1BB2716-FABC-48C8-8345-38A1605476A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1">
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2057400" y="4086225"/>
+          <a:ext cx="647700" cy="1095375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="0" tIns="27432" rIns="36576" bIns="27432" anchor="ctr" upright="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="r" rtl="0">
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Arial"/>
+              <a:cs typeface="Arial"/>
+            </a:rPr>
+            <a:t>Target Dates</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2899,26 +3272,26 @@
       <c r="Y2" s="14"/>
     </row>
     <row r="3" spans="1:25" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="83" t="s">
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="83"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="83"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="104"/>
       <c r="Q3" s="66"/>
       <c r="R3" s="66"/>
       <c r="S3" s="66"/>
@@ -2929,22 +3302,22 @@
       <c r="Y3" s="14"/>
     </row>
     <row r="4" spans="1:25" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81"/>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="84"/>
-      <c r="M4" s="84"/>
-      <c r="N4" s="84"/>
-      <c r="O4" s="84"/>
-      <c r="P4" s="84"/>
+      <c r="A4" s="102"/>
+      <c r="B4" s="103"/>
+      <c r="C4" s="103"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="105"/>
+      <c r="N4" s="105"/>
+      <c r="O4" s="105"/>
+      <c r="P4" s="105"/>
       <c r="Q4" s="68"/>
       <c r="R4" s="68"/>
       <c r="S4" s="68"/>
@@ -2961,27 +3334,27 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="85" t="s">
+      <c r="E5" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="86"/>
-      <c r="L5" s="86"/>
-      <c r="M5" s="86"/>
-      <c r="N5" s="87"/>
-      <c r="O5" s="87"/>
-      <c r="P5" s="88"/>
-      <c r="Q5" s="89" t="s">
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="107"/>
+      <c r="K5" s="107"/>
+      <c r="L5" s="107"/>
+      <c r="M5" s="107"/>
+      <c r="N5" s="108"/>
+      <c r="O5" s="108"/>
+      <c r="P5" s="109"/>
+      <c r="Q5" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="R5" s="86"/>
-      <c r="S5" s="86"/>
-      <c r="T5" s="86"/>
-      <c r="U5" s="88"/>
+      <c r="R5" s="107"/>
+      <c r="S5" s="107"/>
+      <c r="T5" s="107"/>
+      <c r="U5" s="109"/>
       <c r="W5" s="21"/>
       <c r="X5" s="22"/>
       <c r="Y5" s="22"/>
@@ -3673,55 +4046,55 @@
       <c r="B26" s="54"/>
       <c r="C26" s="55"/>
       <c r="D26" s="55"/>
-      <c r="E26" s="109" t="s">
+      <c r="E26" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="90" t="s">
+      <c r="F26" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="90" t="s">
+      <c r="G26" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="H26" s="90" t="s">
+      <c r="H26" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="I26" s="90" t="s">
+      <c r="I26" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="J26" s="90" t="s">
+      <c r="J26" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="K26" s="90" t="s">
+      <c r="K26" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="L26" s="90" t="s">
+      <c r="L26" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="M26" s="90" t="s">
+      <c r="M26" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="N26" s="90" t="s">
+      <c r="N26" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="O26" s="90" t="s">
+      <c r="O26" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="P26" s="100" t="s">
+      <c r="P26" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="Q26" s="107" t="s">
+      <c r="Q26" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="R26" s="98" t="s">
+      <c r="R26" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="S26" s="98" t="s">
+      <c r="S26" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="T26" s="98" t="s">
+      <c r="T26" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="U26" s="105" t="s">
+      <c r="U26" s="94" t="s">
         <v>31</v>
       </c>
       <c r="W26" s="31"/>
@@ -3733,23 +4106,23 @@
       <c r="B27" s="56"/>
       <c r="C27" s="55"/>
       <c r="D27" s="55"/>
-      <c r="E27" s="109"/>
-      <c r="F27" s="90"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="90"/>
-      <c r="I27" s="90"/>
-      <c r="J27" s="90"/>
-      <c r="K27" s="90"/>
-      <c r="L27" s="90"/>
-      <c r="M27" s="90"/>
-      <c r="N27" s="90"/>
-      <c r="O27" s="90"/>
-      <c r="P27" s="100"/>
-      <c r="Q27" s="107"/>
-      <c r="R27" s="98"/>
-      <c r="S27" s="98"/>
-      <c r="T27" s="98"/>
-      <c r="U27" s="105"/>
+      <c r="E27" s="98"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="87"/>
+      <c r="J27" s="87"/>
+      <c r="K27" s="87"/>
+      <c r="L27" s="87"/>
+      <c r="M27" s="87"/>
+      <c r="N27" s="87"/>
+      <c r="O27" s="87"/>
+      <c r="P27" s="89"/>
+      <c r="Q27" s="96"/>
+      <c r="R27" s="85"/>
+      <c r="S27" s="85"/>
+      <c r="T27" s="85"/>
+      <c r="U27" s="94"/>
       <c r="W27" s="31"/>
       <c r="X27" s="32"/>
       <c r="Y27" s="32"/>
@@ -3759,23 +4132,23 @@
       <c r="B28" s="56"/>
       <c r="C28" s="55"/>
       <c r="D28" s="55"/>
-      <c r="E28" s="109"/>
-      <c r="F28" s="90"/>
-      <c r="G28" s="90"/>
-      <c r="H28" s="90"/>
-      <c r="I28" s="90"/>
-      <c r="J28" s="90"/>
-      <c r="K28" s="90"/>
-      <c r="L28" s="90"/>
-      <c r="M28" s="90"/>
-      <c r="N28" s="90"/>
-      <c r="O28" s="90"/>
-      <c r="P28" s="100"/>
-      <c r="Q28" s="107"/>
-      <c r="R28" s="98"/>
-      <c r="S28" s="98"/>
-      <c r="T28" s="98"/>
-      <c r="U28" s="105"/>
+      <c r="E28" s="98"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="87"/>
+      <c r="I28" s="87"/>
+      <c r="J28" s="87"/>
+      <c r="K28" s="87"/>
+      <c r="L28" s="87"/>
+      <c r="M28" s="87"/>
+      <c r="N28" s="87"/>
+      <c r="O28" s="87"/>
+      <c r="P28" s="89"/>
+      <c r="Q28" s="96"/>
+      <c r="R28" s="85"/>
+      <c r="S28" s="85"/>
+      <c r="T28" s="85"/>
+      <c r="U28" s="94"/>
       <c r="W28" s="31"/>
       <c r="X28" s="32"/>
       <c r="Y28" s="32"/>
@@ -3785,23 +4158,23 @@
       <c r="B29" s="57"/>
       <c r="C29" s="55"/>
       <c r="D29" s="55"/>
-      <c r="E29" s="109"/>
-      <c r="F29" s="90"/>
-      <c r="G29" s="90"/>
-      <c r="H29" s="90"/>
-      <c r="I29" s="90"/>
-      <c r="J29" s="90"/>
-      <c r="K29" s="90"/>
-      <c r="L29" s="90"/>
-      <c r="M29" s="90"/>
-      <c r="N29" s="90"/>
-      <c r="O29" s="90"/>
-      <c r="P29" s="100"/>
-      <c r="Q29" s="107"/>
-      <c r="R29" s="98"/>
-      <c r="S29" s="98"/>
-      <c r="T29" s="98"/>
-      <c r="U29" s="105"/>
+      <c r="E29" s="98"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
+      <c r="H29" s="87"/>
+      <c r="I29" s="87"/>
+      <c r="J29" s="87"/>
+      <c r="K29" s="87"/>
+      <c r="L29" s="87"/>
+      <c r="M29" s="87"/>
+      <c r="N29" s="87"/>
+      <c r="O29" s="87"/>
+      <c r="P29" s="89"/>
+      <c r="Q29" s="96"/>
+      <c r="R29" s="85"/>
+      <c r="S29" s="85"/>
+      <c r="T29" s="85"/>
+      <c r="U29" s="94"/>
       <c r="X29" s="32"/>
       <c r="Y29" s="32"/>
     </row>
@@ -3810,23 +4183,23 @@
       <c r="B30" s="54"/>
       <c r="C30" s="55"/>
       <c r="D30" s="55"/>
-      <c r="E30" s="109"/>
-      <c r="F30" s="90"/>
-      <c r="G30" s="90"/>
-      <c r="H30" s="90"/>
-      <c r="I30" s="90"/>
-      <c r="J30" s="90"/>
-      <c r="K30" s="90"/>
-      <c r="L30" s="90"/>
-      <c r="M30" s="90"/>
-      <c r="N30" s="90"/>
-      <c r="O30" s="90"/>
-      <c r="P30" s="100"/>
-      <c r="Q30" s="107"/>
-      <c r="R30" s="98"/>
-      <c r="S30" s="98"/>
-      <c r="T30" s="98"/>
-      <c r="U30" s="105"/>
+      <c r="E30" s="98"/>
+      <c r="F30" s="87"/>
+      <c r="G30" s="87"/>
+      <c r="H30" s="87"/>
+      <c r="I30" s="87"/>
+      <c r="J30" s="87"/>
+      <c r="K30" s="87"/>
+      <c r="L30" s="87"/>
+      <c r="M30" s="87"/>
+      <c r="N30" s="87"/>
+      <c r="O30" s="87"/>
+      <c r="P30" s="89"/>
+      <c r="Q30" s="96"/>
+      <c r="R30" s="85"/>
+      <c r="S30" s="85"/>
+      <c r="T30" s="85"/>
+      <c r="U30" s="94"/>
       <c r="X30" s="32"/>
       <c r="Y30" s="32"/>
     </row>
@@ -3835,126 +4208,126 @@
       <c r="B31" s="58"/>
       <c r="C31" s="55"/>
       <c r="D31" s="55"/>
-      <c r="E31" s="110"/>
-      <c r="F31" s="91"/>
-      <c r="G31" s="91"/>
-      <c r="H31" s="91"/>
-      <c r="I31" s="91"/>
-      <c r="J31" s="91"/>
-      <c r="K31" s="91"/>
-      <c r="L31" s="91"/>
-      <c r="M31" s="91"/>
-      <c r="N31" s="91"/>
-      <c r="O31" s="91"/>
-      <c r="P31" s="101"/>
-      <c r="Q31" s="108"/>
-      <c r="R31" s="99"/>
-      <c r="S31" s="99"/>
-      <c r="T31" s="99"/>
-      <c r="U31" s="106"/>
+      <c r="E31" s="99"/>
+      <c r="F31" s="88"/>
+      <c r="G31" s="88"/>
+      <c r="H31" s="88"/>
+      <c r="I31" s="88"/>
+      <c r="J31" s="88"/>
+      <c r="K31" s="88"/>
+      <c r="L31" s="88"/>
+      <c r="M31" s="88"/>
+      <c r="N31" s="88"/>
+      <c r="O31" s="88"/>
+      <c r="P31" s="90"/>
+      <c r="Q31" s="97"/>
+      <c r="R31" s="86"/>
+      <c r="S31" s="86"/>
+      <c r="T31" s="86"/>
+      <c r="U31" s="95"/>
       <c r="W31" s="21"/>
       <c r="X31" s="21"/>
       <c r="Y31" s="21"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A32" s="102" t="s">
+      <c r="A32" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="103"/>
-      <c r="C32" s="103"/>
-      <c r="D32" s="103"/>
-      <c r="E32" s="103"/>
-      <c r="F32" s="103"/>
-      <c r="G32" s="103"/>
-      <c r="H32" s="103"/>
-      <c r="I32" s="103"/>
-      <c r="J32" s="103"/>
-      <c r="K32" s="103"/>
-      <c r="L32" s="103"/>
-      <c r="M32" s="103"/>
-      <c r="N32" s="103"/>
-      <c r="O32" s="103"/>
-      <c r="P32" s="103"/>
-      <c r="Q32" s="103"/>
-      <c r="R32" s="103"/>
-      <c r="S32" s="103"/>
-      <c r="T32" s="103"/>
-      <c r="U32" s="104"/>
+      <c r="B32" s="92"/>
+      <c r="C32" s="92"/>
+      <c r="D32" s="92"/>
+      <c r="E32" s="92"/>
+      <c r="F32" s="92"/>
+      <c r="G32" s="92"/>
+      <c r="H32" s="92"/>
+      <c r="I32" s="92"/>
+      <c r="J32" s="92"/>
+      <c r="K32" s="92"/>
+      <c r="L32" s="92"/>
+      <c r="M32" s="92"/>
+      <c r="N32" s="92"/>
+      <c r="O32" s="92"/>
+      <c r="P32" s="92"/>
+      <c r="Q32" s="92"/>
+      <c r="R32" s="92"/>
+      <c r="S32" s="92"/>
+      <c r="T32" s="92"/>
+      <c r="U32" s="93"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A33" s="92" t="s">
+      <c r="A33" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="93"/>
-      <c r="C33" s="93"/>
-      <c r="D33" s="93"/>
-      <c r="E33" s="93"/>
-      <c r="F33" s="93"/>
-      <c r="G33" s="93"/>
-      <c r="H33" s="93"/>
-      <c r="I33" s="93"/>
-      <c r="J33" s="93"/>
-      <c r="K33" s="93"/>
-      <c r="L33" s="93"/>
-      <c r="M33" s="93"/>
-      <c r="N33" s="93"/>
-      <c r="O33" s="93"/>
-      <c r="P33" s="93"/>
-      <c r="Q33" s="93"/>
-      <c r="R33" s="93"/>
-      <c r="S33" s="93"/>
-      <c r="T33" s="93"/>
-      <c r="U33" s="94"/>
+      <c r="B33" s="80"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="80"/>
+      <c r="I33" s="80"/>
+      <c r="J33" s="80"/>
+      <c r="K33" s="80"/>
+      <c r="L33" s="80"/>
+      <c r="M33" s="80"/>
+      <c r="N33" s="80"/>
+      <c r="O33" s="80"/>
+      <c r="P33" s="80"/>
+      <c r="Q33" s="80"/>
+      <c r="R33" s="80"/>
+      <c r="S33" s="80"/>
+      <c r="T33" s="80"/>
+      <c r="U33" s="81"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A34" s="92" t="s">
+      <c r="A34" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="93"/>
-      <c r="C34" s="93"/>
-      <c r="D34" s="93"/>
-      <c r="E34" s="93"/>
-      <c r="F34" s="93"/>
-      <c r="G34" s="93"/>
-      <c r="H34" s="93"/>
-      <c r="I34" s="93"/>
-      <c r="J34" s="93"/>
-      <c r="K34" s="93"/>
-      <c r="L34" s="93"/>
-      <c r="M34" s="93"/>
-      <c r="N34" s="93"/>
-      <c r="O34" s="93"/>
-      <c r="P34" s="93"/>
-      <c r="Q34" s="93"/>
-      <c r="R34" s="93"/>
-      <c r="S34" s="93"/>
-      <c r="T34" s="93"/>
-      <c r="U34" s="94"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="80"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="80"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="80"/>
+      <c r="I34" s="80"/>
+      <c r="J34" s="80"/>
+      <c r="K34" s="80"/>
+      <c r="L34" s="80"/>
+      <c r="M34" s="80"/>
+      <c r="N34" s="80"/>
+      <c r="O34" s="80"/>
+      <c r="P34" s="80"/>
+      <c r="Q34" s="80"/>
+      <c r="R34" s="80"/>
+      <c r="S34" s="80"/>
+      <c r="T34" s="80"/>
+      <c r="U34" s="81"/>
     </row>
     <row r="35" spans="1:25" s="18" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="95" t="s">
+      <c r="A35" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="96"/>
-      <c r="C35" s="96"/>
-      <c r="D35" s="96"/>
-      <c r="E35" s="96"/>
-      <c r="F35" s="96"/>
-      <c r="G35" s="96"/>
-      <c r="H35" s="96"/>
-      <c r="I35" s="96"/>
-      <c r="J35" s="96"/>
-      <c r="K35" s="96"/>
-      <c r="L35" s="96"/>
-      <c r="M35" s="96"/>
-      <c r="N35" s="96"/>
-      <c r="O35" s="96"/>
-      <c r="P35" s="96"/>
-      <c r="Q35" s="96"/>
-      <c r="R35" s="96"/>
-      <c r="S35" s="96"/>
-      <c r="T35" s="96"/>
-      <c r="U35" s="97"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="83"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="83"/>
+      <c r="F35" s="83"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="83"/>
+      <c r="I35" s="83"/>
+      <c r="J35" s="83"/>
+      <c r="K35" s="83"/>
+      <c r="L35" s="83"/>
+      <c r="M35" s="83"/>
+      <c r="N35" s="83"/>
+      <c r="O35" s="83"/>
+      <c r="P35" s="83"/>
+      <c r="Q35" s="83"/>
+      <c r="R35" s="83"/>
+      <c r="S35" s="83"/>
+      <c r="T35" s="83"/>
+      <c r="U35" s="84"/>
       <c r="W35" s="21"/>
       <c r="X35" s="22"/>
       <c r="Y35" s="22"/>
@@ -4036,6 +4409,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="E3:P4"/>
+    <mergeCell ref="E5:P5"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="F26:F31"/>
+    <mergeCell ref="G26:G31"/>
+    <mergeCell ref="N26:N31"/>
+    <mergeCell ref="I26:I31"/>
+    <mergeCell ref="J26:J31"/>
     <mergeCell ref="A34:U34"/>
     <mergeCell ref="A35:U35"/>
     <mergeCell ref="T26:T31"/>
@@ -4052,80 +4434,71 @@
     <mergeCell ref="Q26:Q31"/>
     <mergeCell ref="K26:K31"/>
     <mergeCell ref="E26:E31"/>
-    <mergeCell ref="A3:D4"/>
-    <mergeCell ref="E3:P4"/>
-    <mergeCell ref="E5:P5"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="F26:F31"/>
-    <mergeCell ref="G26:G31"/>
-    <mergeCell ref="N26:N31"/>
-    <mergeCell ref="I26:I31"/>
-    <mergeCell ref="J26:J31"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="D38:E38 I38:Y38">
-    <cfRule type="cellIs" dxfId="47" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="26" stopIfTrue="1" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="27" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="27" stopIfTrue="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="28" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="28" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:G6 I6:K6 M6:P6 G7:N7 P7 G8:L8 E9:F9 J9:L9 E10:G10 I10:M10 O10:P10 E11:J11 E12:G12 K12 E13:H13 J13:N13 P13 N14:P14 E14:I15 M15:O15 E16:J16 L16:P16 E17:I17 K17:P17 E18:P25">
-    <cfRule type="cellIs" dxfId="44" priority="29" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="29" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="30" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="30" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="31" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="31" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="41" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="13" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="14" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="15" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="38" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="10" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="11" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="12" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11:P12">
-    <cfRule type="cellIs" dxfId="35" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="1" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="2" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="3" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8:P9">
-    <cfRule type="cellIs" dxfId="32" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="16" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="17" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="18" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4196,26 +4569,26 @@
       <c r="Y2" s="14"/>
     </row>
     <row r="3" spans="1:25" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="83" t="s">
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="83"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="83"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="104"/>
       <c r="Q3" s="66"/>
       <c r="R3" s="66"/>
       <c r="S3" s="66"/>
@@ -4226,22 +4599,22 @@
       <c r="Y3" s="14"/>
     </row>
     <row r="4" spans="1:25" s="15" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="81"/>
-      <c r="B4" s="82"/>
-      <c r="C4" s="82"/>
-      <c r="D4" s="82"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="84"/>
-      <c r="M4" s="84"/>
-      <c r="N4" s="84"/>
-      <c r="O4" s="84"/>
-      <c r="P4" s="84"/>
+      <c r="A4" s="102"/>
+      <c r="B4" s="103"/>
+      <c r="C4" s="103"/>
+      <c r="D4" s="103"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="105"/>
+      <c r="N4" s="105"/>
+      <c r="O4" s="105"/>
+      <c r="P4" s="105"/>
       <c r="Q4" s="68"/>
       <c r="R4" s="68"/>
       <c r="S4" s="68"/>
@@ -4258,27 +4631,27 @@
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="85" t="s">
+      <c r="E5" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
-      <c r="I5" s="86"/>
-      <c r="J5" s="86"/>
-      <c r="K5" s="86"/>
-      <c r="L5" s="86"/>
-      <c r="M5" s="86"/>
-      <c r="N5" s="87"/>
-      <c r="O5" s="87"/>
-      <c r="P5" s="88"/>
-      <c r="Q5" s="89" t="s">
+      <c r="F5" s="107"/>
+      <c r="G5" s="107"/>
+      <c r="H5" s="107"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="107"/>
+      <c r="K5" s="107"/>
+      <c r="L5" s="107"/>
+      <c r="M5" s="107"/>
+      <c r="N5" s="108"/>
+      <c r="O5" s="108"/>
+      <c r="P5" s="109"/>
+      <c r="Q5" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="R5" s="86"/>
-      <c r="S5" s="86"/>
-      <c r="T5" s="86"/>
-      <c r="U5" s="88"/>
+      <c r="R5" s="107"/>
+      <c r="S5" s="107"/>
+      <c r="T5" s="107"/>
+      <c r="U5" s="109"/>
       <c r="W5" s="21"/>
       <c r="X5" s="22"/>
       <c r="Y5" s="22"/>
@@ -4968,55 +5341,55 @@
       <c r="B26" s="54"/>
       <c r="C26" s="55"/>
       <c r="D26" s="55"/>
-      <c r="E26" s="109" t="s">
+      <c r="E26" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="90" t="s">
+      <c r="F26" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="90" t="s">
+      <c r="G26" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="H26" s="90" t="s">
+      <c r="H26" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="I26" s="90" t="s">
+      <c r="I26" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="J26" s="90" t="s">
+      <c r="J26" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="K26" s="90" t="s">
+      <c r="K26" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="L26" s="90" t="s">
+      <c r="L26" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="M26" s="90" t="s">
+      <c r="M26" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="N26" s="90" t="s">
+      <c r="N26" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="O26" s="90" t="s">
+      <c r="O26" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="P26" s="100" t="s">
+      <c r="P26" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="Q26" s="107" t="s">
+      <c r="Q26" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="R26" s="98" t="s">
+      <c r="R26" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="S26" s="98" t="s">
+      <c r="S26" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="T26" s="98" t="s">
+      <c r="T26" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="U26" s="105" t="s">
+      <c r="U26" s="94" t="s">
         <v>31</v>
       </c>
       <c r="W26" s="31"/>
@@ -5028,23 +5401,23 @@
       <c r="B27" s="56"/>
       <c r="C27" s="55"/>
       <c r="D27" s="55"/>
-      <c r="E27" s="109"/>
-      <c r="F27" s="90"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="90"/>
-      <c r="I27" s="90"/>
-      <c r="J27" s="90"/>
-      <c r="K27" s="90"/>
-      <c r="L27" s="90"/>
-      <c r="M27" s="90"/>
-      <c r="N27" s="90"/>
-      <c r="O27" s="90"/>
-      <c r="P27" s="100"/>
-      <c r="Q27" s="107"/>
-      <c r="R27" s="98"/>
-      <c r="S27" s="98"/>
-      <c r="T27" s="98"/>
-      <c r="U27" s="105"/>
+      <c r="E27" s="98"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="87"/>
+      <c r="J27" s="87"/>
+      <c r="K27" s="87"/>
+      <c r="L27" s="87"/>
+      <c r="M27" s="87"/>
+      <c r="N27" s="87"/>
+      <c r="O27" s="87"/>
+      <c r="P27" s="89"/>
+      <c r="Q27" s="96"/>
+      <c r="R27" s="85"/>
+      <c r="S27" s="85"/>
+      <c r="T27" s="85"/>
+      <c r="U27" s="94"/>
       <c r="W27" s="31"/>
       <c r="X27" s="32"/>
       <c r="Y27" s="32"/>
@@ -5054,23 +5427,23 @@
       <c r="B28" s="56"/>
       <c r="C28" s="55"/>
       <c r="D28" s="55"/>
-      <c r="E28" s="109"/>
-      <c r="F28" s="90"/>
-      <c r="G28" s="90"/>
-      <c r="H28" s="90"/>
-      <c r="I28" s="90"/>
-      <c r="J28" s="90"/>
-      <c r="K28" s="90"/>
-      <c r="L28" s="90"/>
-      <c r="M28" s="90"/>
-      <c r="N28" s="90"/>
-      <c r="O28" s="90"/>
-      <c r="P28" s="100"/>
-      <c r="Q28" s="107"/>
-      <c r="R28" s="98"/>
-      <c r="S28" s="98"/>
-      <c r="T28" s="98"/>
-      <c r="U28" s="105"/>
+      <c r="E28" s="98"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="87"/>
+      <c r="I28" s="87"/>
+      <c r="J28" s="87"/>
+      <c r="K28" s="87"/>
+      <c r="L28" s="87"/>
+      <c r="M28" s="87"/>
+      <c r="N28" s="87"/>
+      <c r="O28" s="87"/>
+      <c r="P28" s="89"/>
+      <c r="Q28" s="96"/>
+      <c r="R28" s="85"/>
+      <c r="S28" s="85"/>
+      <c r="T28" s="85"/>
+      <c r="U28" s="94"/>
       <c r="W28" s="31"/>
       <c r="X28" s="32"/>
       <c r="Y28" s="32"/>
@@ -5080,23 +5453,23 @@
       <c r="B29" s="57"/>
       <c r="C29" s="55"/>
       <c r="D29" s="55"/>
-      <c r="E29" s="109"/>
-      <c r="F29" s="90"/>
-      <c r="G29" s="90"/>
-      <c r="H29" s="90"/>
-      <c r="I29" s="90"/>
-      <c r="J29" s="90"/>
-      <c r="K29" s="90"/>
-      <c r="L29" s="90"/>
-      <c r="M29" s="90"/>
-      <c r="N29" s="90"/>
-      <c r="O29" s="90"/>
-      <c r="P29" s="100"/>
-      <c r="Q29" s="107"/>
-      <c r="R29" s="98"/>
-      <c r="S29" s="98"/>
-      <c r="T29" s="98"/>
-      <c r="U29" s="105"/>
+      <c r="E29" s="98"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
+      <c r="H29" s="87"/>
+      <c r="I29" s="87"/>
+      <c r="J29" s="87"/>
+      <c r="K29" s="87"/>
+      <c r="L29" s="87"/>
+      <c r="M29" s="87"/>
+      <c r="N29" s="87"/>
+      <c r="O29" s="87"/>
+      <c r="P29" s="89"/>
+      <c r="Q29" s="96"/>
+      <c r="R29" s="85"/>
+      <c r="S29" s="85"/>
+      <c r="T29" s="85"/>
+      <c r="U29" s="94"/>
       <c r="X29" s="32"/>
       <c r="Y29" s="32"/>
     </row>
@@ -5105,23 +5478,23 @@
       <c r="B30" s="54"/>
       <c r="C30" s="55"/>
       <c r="D30" s="55"/>
-      <c r="E30" s="109"/>
-      <c r="F30" s="90"/>
-      <c r="G30" s="90"/>
-      <c r="H30" s="90"/>
-      <c r="I30" s="90"/>
-      <c r="J30" s="90"/>
-      <c r="K30" s="90"/>
-      <c r="L30" s="90"/>
-      <c r="M30" s="90"/>
-      <c r="N30" s="90"/>
-      <c r="O30" s="90"/>
-      <c r="P30" s="100"/>
-      <c r="Q30" s="107"/>
-      <c r="R30" s="98"/>
-      <c r="S30" s="98"/>
-      <c r="T30" s="98"/>
-      <c r="U30" s="105"/>
+      <c r="E30" s="98"/>
+      <c r="F30" s="87"/>
+      <c r="G30" s="87"/>
+      <c r="H30" s="87"/>
+      <c r="I30" s="87"/>
+      <c r="J30" s="87"/>
+      <c r="K30" s="87"/>
+      <c r="L30" s="87"/>
+      <c r="M30" s="87"/>
+      <c r="N30" s="87"/>
+      <c r="O30" s="87"/>
+      <c r="P30" s="89"/>
+      <c r="Q30" s="96"/>
+      <c r="R30" s="85"/>
+      <c r="S30" s="85"/>
+      <c r="T30" s="85"/>
+      <c r="U30" s="94"/>
       <c r="X30" s="32"/>
       <c r="Y30" s="32"/>
     </row>
@@ -5130,23 +5503,23 @@
       <c r="B31" s="58"/>
       <c r="C31" s="55"/>
       <c r="D31" s="55"/>
-      <c r="E31" s="110"/>
-      <c r="F31" s="91"/>
-      <c r="G31" s="91"/>
-      <c r="H31" s="91"/>
-      <c r="I31" s="91"/>
-      <c r="J31" s="91"/>
-      <c r="K31" s="91"/>
-      <c r="L31" s="91"/>
-      <c r="M31" s="91"/>
-      <c r="N31" s="91"/>
-      <c r="O31" s="91"/>
-      <c r="P31" s="101"/>
-      <c r="Q31" s="108"/>
-      <c r="R31" s="99"/>
-      <c r="S31" s="99"/>
-      <c r="T31" s="99"/>
-      <c r="U31" s="106"/>
+      <c r="E31" s="99"/>
+      <c r="F31" s="88"/>
+      <c r="G31" s="88"/>
+      <c r="H31" s="88"/>
+      <c r="I31" s="88"/>
+      <c r="J31" s="88"/>
+      <c r="K31" s="88"/>
+      <c r="L31" s="88"/>
+      <c r="M31" s="88"/>
+      <c r="N31" s="88"/>
+      <c r="O31" s="88"/>
+      <c r="P31" s="90"/>
+      <c r="Q31" s="97"/>
+      <c r="R31" s="86"/>
+      <c r="S31" s="86"/>
+      <c r="T31" s="86"/>
+      <c r="U31" s="95"/>
       <c r="W31" s="21"/>
       <c r="X31" s="21"/>
       <c r="Y31" s="21"/>
@@ -5155,101 +5528,101 @@
       <c r="A32" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="B32" s="103"/>
-      <c r="C32" s="103"/>
-      <c r="D32" s="103"/>
-      <c r="E32" s="103"/>
-      <c r="F32" s="103"/>
-      <c r="G32" s="103"/>
-      <c r="H32" s="103"/>
-      <c r="I32" s="103"/>
-      <c r="J32" s="103"/>
-      <c r="K32" s="103"/>
-      <c r="L32" s="103"/>
-      <c r="M32" s="103"/>
-      <c r="N32" s="103"/>
-      <c r="O32" s="103"/>
-      <c r="P32" s="103"/>
-      <c r="Q32" s="103"/>
-      <c r="R32" s="103"/>
-      <c r="S32" s="103"/>
-      <c r="T32" s="103"/>
-      <c r="U32" s="104"/>
+      <c r="B32" s="92"/>
+      <c r="C32" s="92"/>
+      <c r="D32" s="92"/>
+      <c r="E32" s="92"/>
+      <c r="F32" s="92"/>
+      <c r="G32" s="92"/>
+      <c r="H32" s="92"/>
+      <c r="I32" s="92"/>
+      <c r="J32" s="92"/>
+      <c r="K32" s="92"/>
+      <c r="L32" s="92"/>
+      <c r="M32" s="92"/>
+      <c r="N32" s="92"/>
+      <c r="O32" s="92"/>
+      <c r="P32" s="92"/>
+      <c r="Q32" s="92"/>
+      <c r="R32" s="92"/>
+      <c r="S32" s="92"/>
+      <c r="T32" s="92"/>
+      <c r="U32" s="93"/>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="111" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="93"/>
-      <c r="C33" s="93"/>
-      <c r="D33" s="93"/>
-      <c r="E33" s="93"/>
-      <c r="F33" s="93"/>
-      <c r="G33" s="93"/>
-      <c r="H33" s="93"/>
-      <c r="I33" s="93"/>
-      <c r="J33" s="93"/>
-      <c r="K33" s="93"/>
-      <c r="L33" s="93"/>
-      <c r="M33" s="93"/>
-      <c r="N33" s="93"/>
-      <c r="O33" s="93"/>
-      <c r="P33" s="93"/>
-      <c r="Q33" s="93"/>
-      <c r="R33" s="93"/>
-      <c r="S33" s="93"/>
-      <c r="T33" s="93"/>
-      <c r="U33" s="94"/>
+      <c r="B33" s="80"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="80"/>
+      <c r="I33" s="80"/>
+      <c r="J33" s="80"/>
+      <c r="K33" s="80"/>
+      <c r="L33" s="80"/>
+      <c r="M33" s="80"/>
+      <c r="N33" s="80"/>
+      <c r="O33" s="80"/>
+      <c r="P33" s="80"/>
+      <c r="Q33" s="80"/>
+      <c r="R33" s="80"/>
+      <c r="S33" s="80"/>
+      <c r="T33" s="80"/>
+      <c r="U33" s="81"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="111" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="93"/>
-      <c r="C34" s="93"/>
-      <c r="D34" s="93"/>
-      <c r="E34" s="93"/>
-      <c r="F34" s="93"/>
-      <c r="G34" s="93"/>
-      <c r="H34" s="93"/>
-      <c r="I34" s="93"/>
-      <c r="J34" s="93"/>
-      <c r="K34" s="93"/>
-      <c r="L34" s="93"/>
-      <c r="M34" s="93"/>
-      <c r="N34" s="93"/>
-      <c r="O34" s="93"/>
-      <c r="P34" s="93"/>
-      <c r="Q34" s="93"/>
-      <c r="R34" s="93"/>
-      <c r="S34" s="93"/>
-      <c r="T34" s="93"/>
-      <c r="U34" s="94"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="80"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="80"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="80"/>
+      <c r="H34" s="80"/>
+      <c r="I34" s="80"/>
+      <c r="J34" s="80"/>
+      <c r="K34" s="80"/>
+      <c r="L34" s="80"/>
+      <c r="M34" s="80"/>
+      <c r="N34" s="80"/>
+      <c r="O34" s="80"/>
+      <c r="P34" s="80"/>
+      <c r="Q34" s="80"/>
+      <c r="R34" s="80"/>
+      <c r="S34" s="80"/>
+      <c r="T34" s="80"/>
+      <c r="U34" s="81"/>
     </row>
     <row r="35" spans="1:25" s="18" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="95" t="s">
+      <c r="A35" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="96"/>
-      <c r="C35" s="96"/>
-      <c r="D35" s="96"/>
-      <c r="E35" s="96"/>
-      <c r="F35" s="96"/>
-      <c r="G35" s="96"/>
-      <c r="H35" s="96"/>
-      <c r="I35" s="96"/>
-      <c r="J35" s="96"/>
-      <c r="K35" s="96"/>
-      <c r="L35" s="96"/>
-      <c r="M35" s="96"/>
-      <c r="N35" s="96"/>
-      <c r="O35" s="96"/>
-      <c r="P35" s="96"/>
-      <c r="Q35" s="96"/>
-      <c r="R35" s="96"/>
-      <c r="S35" s="96"/>
-      <c r="T35" s="96"/>
-      <c r="U35" s="97"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="83"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="83"/>
+      <c r="F35" s="83"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="83"/>
+      <c r="I35" s="83"/>
+      <c r="J35" s="83"/>
+      <c r="K35" s="83"/>
+      <c r="L35" s="83"/>
+      <c r="M35" s="83"/>
+      <c r="N35" s="83"/>
+      <c r="O35" s="83"/>
+      <c r="P35" s="83"/>
+      <c r="Q35" s="83"/>
+      <c r="R35" s="83"/>
+      <c r="S35" s="83"/>
+      <c r="T35" s="83"/>
+      <c r="U35" s="84"/>
       <c r="W35" s="21"/>
       <c r="X35" s="22"/>
       <c r="Y35" s="22"/>
@@ -5331,16 +5704,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A3:D4"/>
-    <mergeCell ref="E3:P4"/>
-    <mergeCell ref="E5:P5"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="E26:E31"/>
-    <mergeCell ref="F26:F31"/>
-    <mergeCell ref="G26:G31"/>
-    <mergeCell ref="H26:H31"/>
-    <mergeCell ref="I26:I31"/>
-    <mergeCell ref="J26:J31"/>
     <mergeCell ref="A33:U33"/>
     <mergeCell ref="A34:U34"/>
     <mergeCell ref="A35:U35"/>
@@ -5356,59 +5719,69 @@
     <mergeCell ref="N26:N31"/>
     <mergeCell ref="O26:O31"/>
     <mergeCell ref="P26:P31"/>
+    <mergeCell ref="A3:D4"/>
+    <mergeCell ref="E3:P4"/>
+    <mergeCell ref="E5:P5"/>
+    <mergeCell ref="Q5:U5"/>
+    <mergeCell ref="E26:E31"/>
+    <mergeCell ref="F26:F31"/>
+    <mergeCell ref="G26:G31"/>
+    <mergeCell ref="H26:H31"/>
+    <mergeCell ref="I26:I31"/>
+    <mergeCell ref="J26:J31"/>
   </mergeCells>
   <conditionalFormatting sqref="D38:E38 I38:Y38">
-    <cfRule type="cellIs" dxfId="29" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="13" stopIfTrue="1" operator="equal">
       <formula>"G"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="14" stopIfTrue="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="15" stopIfTrue="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6:G6 I6:K6 M6:P6 P7 G7:L8 E9:F9 J9:L9 K12 P12 E12:G13 I13:L13 O13:P13 E14:J14 M14:P14 E15:H15 J15:N15 P15 N16:P16 E16:I17 M17:O17 E18:J18 L18:P18 E19:I19 K19:L19 E21:P25">
-    <cfRule type="cellIs" dxfId="26" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="16" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="17" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="18" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="23" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="7" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="8" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="9" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="20" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="4" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="5" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="6" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N8:P8 P9">
-    <cfRule type="cellIs" dxfId="17" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="10" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="11" stopIfTrue="1" operator="equal">
       <formula>"C"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="12" stopIfTrue="1" operator="equal">
       <formula>"D"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5422,8 +5795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50661F68-A50F-4C74-B3DE-EB252B9D0F85}">
   <dimension ref="A1:U37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView topLeftCell="C14" workbookViewId="0">
+      <selection sqref="A1:U37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5458,26 +5831,26 @@
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="83" t="s">
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
       <c r="Q2" s="66"/>
       <c r="R2" s="66"/>
       <c r="S2" s="66"/>
@@ -5485,22 +5858,22 @@
       <c r="U2" s="67"/>
     </row>
     <row r="3" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="81"/>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="82"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="84"/>
-      <c r="N3" s="84"/>
-      <c r="O3" s="84"/>
-      <c r="P3" s="84"/>
+      <c r="A3" s="102"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105"/>
+      <c r="M3" s="105"/>
+      <c r="N3" s="105"/>
+      <c r="O3" s="105"/>
+      <c r="P3" s="105"/>
       <c r="Q3" s="68"/>
       <c r="R3" s="68"/>
       <c r="S3" s="68"/>
@@ -5514,27 +5887,27 @@
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
-      <c r="E4" s="85" t="s">
+      <c r="E4" s="106" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
-      <c r="I4" s="86"/>
-      <c r="J4" s="86"/>
-      <c r="K4" s="86"/>
-      <c r="L4" s="86"/>
-      <c r="M4" s="86"/>
-      <c r="N4" s="87"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="88"/>
-      <c r="Q4" s="89" t="s">
+      <c r="F4" s="107"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="107"/>
+      <c r="I4" s="107"/>
+      <c r="J4" s="107"/>
+      <c r="K4" s="107"/>
+      <c r="L4" s="107"/>
+      <c r="M4" s="107"/>
+      <c r="N4" s="108"/>
+      <c r="O4" s="108"/>
+      <c r="P4" s="109"/>
+      <c r="Q4" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="86"/>
-      <c r="S4" s="86"/>
-      <c r="T4" s="86"/>
-      <c r="U4" s="88"/>
+      <c r="R4" s="107"/>
+      <c r="S4" s="107"/>
+      <c r="T4" s="107"/>
+      <c r="U4" s="109"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="24">
@@ -6241,55 +6614,55 @@
       <c r="B25" s="54"/>
       <c r="C25" s="55"/>
       <c r="D25" s="55"/>
-      <c r="E25" s="109" t="s">
+      <c r="E25" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="90" t="s">
+      <c r="F25" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="90" t="s">
+      <c r="G25" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="H25" s="90" t="s">
+      <c r="H25" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="I25" s="90" t="s">
+      <c r="I25" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="J25" s="90" t="s">
+      <c r="J25" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="90" t="s">
+      <c r="K25" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="L25" s="90" t="s">
+      <c r="L25" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="M25" s="90" t="s">
+      <c r="M25" s="87" t="s">
         <v>15</v>
       </c>
-      <c r="N25" s="90" t="s">
+      <c r="N25" s="87" t="s">
         <v>16</v>
       </c>
-      <c r="O25" s="90" t="s">
+      <c r="O25" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="P25" s="100" t="s">
+      <c r="P25" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="Q25" s="107" t="s">
+      <c r="Q25" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="R25" s="98" t="s">
+      <c r="R25" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="S25" s="98" t="s">
+      <c r="S25" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="T25" s="98" t="s">
+      <c r="T25" s="85" t="s">
         <v>30</v>
       </c>
-      <c r="U25" s="105" t="s">
+      <c r="U25" s="94" t="s">
         <v>31</v>
       </c>
     </row>
@@ -6298,213 +6671,1478 @@
       <c r="B26" s="56"/>
       <c r="C26" s="55"/>
       <c r="D26" s="55"/>
-      <c r="E26" s="109"/>
-      <c r="F26" s="90"/>
-      <c r="G26" s="90"/>
-      <c r="H26" s="90"/>
-      <c r="I26" s="90"/>
-      <c r="J26" s="90"/>
-      <c r="K26" s="90"/>
-      <c r="L26" s="90"/>
-      <c r="M26" s="90"/>
-      <c r="N26" s="90"/>
-      <c r="O26" s="90"/>
-      <c r="P26" s="100"/>
-      <c r="Q26" s="107"/>
-      <c r="R26" s="98"/>
-      <c r="S26" s="98"/>
-      <c r="T26" s="98"/>
-      <c r="U26" s="105"/>
+      <c r="E26" s="98"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="87"/>
+      <c r="I26" s="87"/>
+      <c r="J26" s="87"/>
+      <c r="K26" s="87"/>
+      <c r="L26" s="87"/>
+      <c r="M26" s="87"/>
+      <c r="N26" s="87"/>
+      <c r="O26" s="87"/>
+      <c r="P26" s="89"/>
+      <c r="Q26" s="96"/>
+      <c r="R26" s="85"/>
+      <c r="S26" s="85"/>
+      <c r="T26" s="85"/>
+      <c r="U26" s="94"/>
     </row>
     <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="53"/>
       <c r="B27" s="56"/>
       <c r="C27" s="55"/>
       <c r="D27" s="55"/>
-      <c r="E27" s="109"/>
-      <c r="F27" s="90"/>
-      <c r="G27" s="90"/>
-      <c r="H27" s="90"/>
-      <c r="I27" s="90"/>
-      <c r="J27" s="90"/>
-      <c r="K27" s="90"/>
-      <c r="L27" s="90"/>
-      <c r="M27" s="90"/>
-      <c r="N27" s="90"/>
-      <c r="O27" s="90"/>
-      <c r="P27" s="100"/>
-      <c r="Q27" s="107"/>
-      <c r="R27" s="98"/>
-      <c r="S27" s="98"/>
-      <c r="T27" s="98"/>
-      <c r="U27" s="105"/>
+      <c r="E27" s="98"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="87"/>
+      <c r="J27" s="87"/>
+      <c r="K27" s="87"/>
+      <c r="L27" s="87"/>
+      <c r="M27" s="87"/>
+      <c r="N27" s="87"/>
+      <c r="O27" s="87"/>
+      <c r="P27" s="89"/>
+      <c r="Q27" s="96"/>
+      <c r="R27" s="85"/>
+      <c r="S27" s="85"/>
+      <c r="T27" s="85"/>
+      <c r="U27" s="94"/>
     </row>
     <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="53"/>
       <c r="B28" s="57"/>
       <c r="C28" s="55"/>
       <c r="D28" s="55"/>
-      <c r="E28" s="109"/>
-      <c r="F28" s="90"/>
-      <c r="G28" s="90"/>
-      <c r="H28" s="90"/>
-      <c r="I28" s="90"/>
-      <c r="J28" s="90"/>
-      <c r="K28" s="90"/>
-      <c r="L28" s="90"/>
-      <c r="M28" s="90"/>
-      <c r="N28" s="90"/>
-      <c r="O28" s="90"/>
-      <c r="P28" s="100"/>
-      <c r="Q28" s="107"/>
-      <c r="R28" s="98"/>
-      <c r="S28" s="98"/>
-      <c r="T28" s="98"/>
-      <c r="U28" s="105"/>
+      <c r="E28" s="98"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="87"/>
+      <c r="I28" s="87"/>
+      <c r="J28" s="87"/>
+      <c r="K28" s="87"/>
+      <c r="L28" s="87"/>
+      <c r="M28" s="87"/>
+      <c r="N28" s="87"/>
+      <c r="O28" s="87"/>
+      <c r="P28" s="89"/>
+      <c r="Q28" s="96"/>
+      <c r="R28" s="85"/>
+      <c r="S28" s="85"/>
+      <c r="T28" s="85"/>
+      <c r="U28" s="94"/>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="53"/>
       <c r="B29" s="54"/>
       <c r="C29" s="55"/>
       <c r="D29" s="55"/>
-      <c r="E29" s="109"/>
-      <c r="F29" s="90"/>
-      <c r="G29" s="90"/>
-      <c r="H29" s="90"/>
-      <c r="I29" s="90"/>
-      <c r="J29" s="90"/>
-      <c r="K29" s="90"/>
-      <c r="L29" s="90"/>
-      <c r="M29" s="90"/>
-      <c r="N29" s="90"/>
-      <c r="O29" s="90"/>
-      <c r="P29" s="100"/>
-      <c r="Q29" s="107"/>
-      <c r="R29" s="98"/>
-      <c r="S29" s="98"/>
-      <c r="T29" s="98"/>
-      <c r="U29" s="105"/>
+      <c r="E29" s="98"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
+      <c r="H29" s="87"/>
+      <c r="I29" s="87"/>
+      <c r="J29" s="87"/>
+      <c r="K29" s="87"/>
+      <c r="L29" s="87"/>
+      <c r="M29" s="87"/>
+      <c r="N29" s="87"/>
+      <c r="O29" s="87"/>
+      <c r="P29" s="89"/>
+      <c r="Q29" s="96"/>
+      <c r="R29" s="85"/>
+      <c r="S29" s="85"/>
+      <c r="T29" s="85"/>
+      <c r="U29" s="94"/>
     </row>
     <row r="30" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="53"/>
       <c r="B30" s="58"/>
       <c r="C30" s="55"/>
       <c r="D30" s="55"/>
-      <c r="E30" s="110"/>
-      <c r="F30" s="91"/>
-      <c r="G30" s="91"/>
-      <c r="H30" s="91"/>
-      <c r="I30" s="91"/>
-      <c r="J30" s="91"/>
-      <c r="K30" s="91"/>
-      <c r="L30" s="91"/>
-      <c r="M30" s="91"/>
-      <c r="N30" s="91"/>
-      <c r="O30" s="91"/>
-      <c r="P30" s="101"/>
-      <c r="Q30" s="108"/>
-      <c r="R30" s="99"/>
-      <c r="S30" s="99"/>
-      <c r="T30" s="99"/>
-      <c r="U30" s="106"/>
+      <c r="E30" s="99"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="88"/>
+      <c r="H30" s="88"/>
+      <c r="I30" s="88"/>
+      <c r="J30" s="88"/>
+      <c r="K30" s="88"/>
+      <c r="L30" s="88"/>
+      <c r="M30" s="88"/>
+      <c r="N30" s="88"/>
+      <c r="O30" s="88"/>
+      <c r="P30" s="90"/>
+      <c r="Q30" s="97"/>
+      <c r="R30" s="86"/>
+      <c r="S30" s="86"/>
+      <c r="T30" s="86"/>
+      <c r="U30" s="95"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="112" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="103"/>
-      <c r="C31" s="103"/>
-      <c r="D31" s="103"/>
-      <c r="E31" s="103"/>
-      <c r="F31" s="103"/>
-      <c r="G31" s="103"/>
-      <c r="H31" s="103"/>
-      <c r="I31" s="103"/>
-      <c r="J31" s="103"/>
-      <c r="K31" s="103"/>
-      <c r="L31" s="103"/>
-      <c r="M31" s="103"/>
-      <c r="N31" s="103"/>
-      <c r="O31" s="103"/>
-      <c r="P31" s="103"/>
-      <c r="Q31" s="103"/>
-      <c r="R31" s="103"/>
-      <c r="S31" s="103"/>
-      <c r="T31" s="103"/>
-      <c r="U31" s="104"/>
+      <c r="B31" s="92"/>
+      <c r="C31" s="92"/>
+      <c r="D31" s="92"/>
+      <c r="E31" s="92"/>
+      <c r="F31" s="92"/>
+      <c r="G31" s="92"/>
+      <c r="H31" s="92"/>
+      <c r="I31" s="92"/>
+      <c r="J31" s="92"/>
+      <c r="K31" s="92"/>
+      <c r="L31" s="92"/>
+      <c r="M31" s="92"/>
+      <c r="N31" s="92"/>
+      <c r="O31" s="92"/>
+      <c r="P31" s="92"/>
+      <c r="Q31" s="92"/>
+      <c r="R31" s="92"/>
+      <c r="S31" s="92"/>
+      <c r="T31" s="92"/>
+      <c r="U31" s="93"/>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A32" s="111" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="93"/>
-      <c r="C32" s="93"/>
-      <c r="D32" s="93"/>
-      <c r="E32" s="93"/>
-      <c r="F32" s="93"/>
-      <c r="G32" s="93"/>
-      <c r="H32" s="93"/>
-      <c r="I32" s="93"/>
-      <c r="J32" s="93"/>
-      <c r="K32" s="93"/>
-      <c r="L32" s="93"/>
-      <c r="M32" s="93"/>
-      <c r="N32" s="93"/>
-      <c r="O32" s="93"/>
-      <c r="P32" s="93"/>
-      <c r="Q32" s="93"/>
-      <c r="R32" s="93"/>
-      <c r="S32" s="93"/>
-      <c r="T32" s="93"/>
-      <c r="U32" s="94"/>
+      <c r="B32" s="80"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="80"/>
+      <c r="I32" s="80"/>
+      <c r="J32" s="80"/>
+      <c r="K32" s="80"/>
+      <c r="L32" s="80"/>
+      <c r="M32" s="80"/>
+      <c r="N32" s="80"/>
+      <c r="O32" s="80"/>
+      <c r="P32" s="80"/>
+      <c r="Q32" s="80"/>
+      <c r="R32" s="80"/>
+      <c r="S32" s="80"/>
+      <c r="T32" s="80"/>
+      <c r="U32" s="81"/>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A33" s="111" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="93"/>
-      <c r="C33" s="93"/>
-      <c r="D33" s="93"/>
-      <c r="E33" s="93"/>
-      <c r="F33" s="93"/>
-      <c r="G33" s="93"/>
-      <c r="H33" s="93"/>
-      <c r="I33" s="93"/>
-      <c r="J33" s="93"/>
-      <c r="K33" s="93"/>
-      <c r="L33" s="93"/>
-      <c r="M33" s="93"/>
-      <c r="N33" s="93"/>
-      <c r="O33" s="93"/>
-      <c r="P33" s="93"/>
-      <c r="Q33" s="93"/>
-      <c r="R33" s="93"/>
-      <c r="S33" s="93"/>
-      <c r="T33" s="93"/>
-      <c r="U33" s="94"/>
+      <c r="B33" s="80"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="80"/>
+      <c r="I33" s="80"/>
+      <c r="J33" s="80"/>
+      <c r="K33" s="80"/>
+      <c r="L33" s="80"/>
+      <c r="M33" s="80"/>
+      <c r="N33" s="80"/>
+      <c r="O33" s="80"/>
+      <c r="P33" s="80"/>
+      <c r="Q33" s="80"/>
+      <c r="R33" s="80"/>
+      <c r="S33" s="80"/>
+      <c r="T33" s="80"/>
+      <c r="U33" s="81"/>
     </row>
     <row r="34" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="95"/>
-      <c r="B34" s="96"/>
-      <c r="C34" s="96"/>
-      <c r="D34" s="96"/>
-      <c r="E34" s="96"/>
-      <c r="F34" s="96"/>
-      <c r="G34" s="96"/>
-      <c r="H34" s="96"/>
-      <c r="I34" s="96"/>
-      <c r="J34" s="96"/>
-      <c r="K34" s="96"/>
-      <c r="L34" s="96"/>
-      <c r="M34" s="96"/>
-      <c r="N34" s="96"/>
-      <c r="O34" s="96"/>
-      <c r="P34" s="96"/>
-      <c r="Q34" s="96"/>
-      <c r="R34" s="96"/>
-      <c r="S34" s="96"/>
-      <c r="T34" s="96"/>
-      <c r="U34" s="97"/>
+      <c r="A34" s="82"/>
+      <c r="B34" s="83"/>
+      <c r="C34" s="83"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="83"/>
+      <c r="F34" s="83"/>
+      <c r="G34" s="83"/>
+      <c r="H34" s="83"/>
+      <c r="I34" s="83"/>
+      <c r="J34" s="83"/>
+      <c r="K34" s="83"/>
+      <c r="L34" s="83"/>
+      <c r="M34" s="83"/>
+      <c r="N34" s="83"/>
+      <c r="O34" s="83"/>
+      <c r="P34" s="83"/>
+      <c r="Q34" s="83"/>
+      <c r="R34" s="83"/>
+      <c r="S34" s="83"/>
+      <c r="T34" s="83"/>
+      <c r="U34" s="84"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
+      <c r="P35" s="18"/>
+      <c r="Q35" s="18"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="18"/>
+      <c r="U35" s="18"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" s="59">
+        <v>152</v>
+      </c>
+      <c r="H36" s="63">
+        <v>153</v>
+      </c>
+      <c r="I36" s="64"/>
+      <c r="J36" s="64"/>
+      <c r="K36" s="60"/>
+      <c r="L36" s="60"/>
+      <c r="M36" s="60"/>
+      <c r="N36" s="60"/>
+      <c r="O36" s="60"/>
+      <c r="P36" s="60"/>
+      <c r="Q36" s="60"/>
+      <c r="R36" s="60"/>
+      <c r="S36" s="60"/>
+      <c r="T36" s="60"/>
+      <c r="U36" s="60"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G37" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="H37" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="I37" s="61"/>
+      <c r="J37" s="61"/>
+      <c r="K37" s="61"/>
+      <c r="L37" s="61"/>
+      <c r="M37" s="61"/>
+      <c r="N37" s="61"/>
+      <c r="O37" s="61"/>
+      <c r="P37" s="61"/>
+      <c r="Q37" s="61"/>
+      <c r="R37" s="61"/>
+      <c r="S37" s="61"/>
+      <c r="T37" s="61"/>
+      <c r="U37" s="61"/>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="A2:D3"/>
+    <mergeCell ref="E2:P3"/>
+    <mergeCell ref="E4:P4"/>
+    <mergeCell ref="Q4:U4"/>
+    <mergeCell ref="E25:E30"/>
+    <mergeCell ref="F25:F30"/>
+    <mergeCell ref="G25:G30"/>
+    <mergeCell ref="H25:H30"/>
+    <mergeCell ref="I25:I30"/>
+    <mergeCell ref="J25:J30"/>
+    <mergeCell ref="A32:U32"/>
+    <mergeCell ref="A33:U33"/>
+    <mergeCell ref="A34:U34"/>
+    <mergeCell ref="Q25:Q30"/>
+    <mergeCell ref="R25:R30"/>
+    <mergeCell ref="S25:S30"/>
+    <mergeCell ref="T25:T30"/>
+    <mergeCell ref="U25:U30"/>
+    <mergeCell ref="A31:U31"/>
+    <mergeCell ref="K25:K30"/>
+    <mergeCell ref="L25:L30"/>
+    <mergeCell ref="M25:M30"/>
+    <mergeCell ref="N25:N30"/>
+    <mergeCell ref="O25:O30"/>
+    <mergeCell ref="P25:P30"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D37:E37 I37:U37">
+    <cfRule type="cellIs" dxfId="29" priority="10" stopIfTrue="1" operator="equal">
+      <formula>"G"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="11" stopIfTrue="1" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:G5 I5:K5 M5:P5 P6 G6:L7 E8:F8 J8:L8 K11 P11 E11:G12 I12:L12 O12:P12 E13:J13 M13:P13 E14:H14 J14:N14 P14 N15:P15 E15:I16 M16:O16 E17:J17 L17:P17 E18:I18 K18:L18 E20:M20 E21:P24">
+    <cfRule type="cellIs" dxfId="26" priority="13" stopIfTrue="1" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="14" stopIfTrue="1" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="15" stopIfTrue="1" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H8">
+    <cfRule type="cellIs" dxfId="23" priority="4" stopIfTrue="1" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="5" stopIfTrue="1" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="6" stopIfTrue="1" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I11">
+    <cfRule type="cellIs" dxfId="20" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="2" stopIfTrue="1" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="3" stopIfTrue="1" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N7:P7 P8">
+    <cfRule type="cellIs" dxfId="17" priority="7" stopIfTrue="1" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="8" stopIfTrue="1" operator="equal">
+      <formula>"C"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="9" stopIfTrue="1" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB11B292-3785-4823-ABF1-D2BA33AA69F2}">
+  <dimension ref="A1:U37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="100" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="104" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
+      <c r="U2" s="67"/>
+    </row>
+    <row r="3" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="102"/>
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="105"/>
+      <c r="F3" s="105"/>
+      <c r="G3" s="105"/>
+      <c r="H3" s="105"/>
+      <c r="I3" s="105"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105"/>
+      <c r="M3" s="105"/>
+      <c r="N3" s="105"/>
+      <c r="O3" s="105"/>
+      <c r="P3" s="105"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="69"/>
+    </row>
+    <row r="4" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="106" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="107"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="107"/>
+      <c r="I4" s="107"/>
+      <c r="J4" s="107"/>
+      <c r="K4" s="107"/>
+      <c r="L4" s="107"/>
+      <c r="M4" s="107"/>
+      <c r="N4" s="108"/>
+      <c r="O4" s="108"/>
+      <c r="P4" s="109"/>
+      <c r="Q4" s="110" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" s="107"/>
+      <c r="S4" s="107"/>
+      <c r="T4" s="107"/>
+      <c r="U4" s="109"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" s="24">
+        <v>1</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="70"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="74" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
+      <c r="O5" s="27"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S5" s="29"/>
+      <c r="T5" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U5" s="30"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" s="33">
+        <v>2</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="N6" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" s="38"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S6" s="40"/>
+      <c r="T6" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U6" s="41"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" s="33">
+        <v>3</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="36" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="41"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" s="33">
+        <v>4</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" s="37"/>
+      <c r="I8" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="N8" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="O8" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="P8" s="38"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="40"/>
+      <c r="S8" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="T8" s="40"/>
+      <c r="U8" s="41"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="N9" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="O9" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9" s="78"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="78"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="O10" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P10" s="78"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="78"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11" s="33">
+        <v>4.3</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="37"/>
+      <c r="J11" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="37"/>
+      <c r="L11" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="M11" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="O11" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="40"/>
+      <c r="S11" s="40"/>
+      <c r="T11" s="40"/>
+      <c r="U11" s="41"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" s="33">
+        <v>5</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="N12" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="O12" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="39"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="40"/>
+      <c r="T12" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U12" s="41"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" s="33">
+        <v>6</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="L13" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="R13" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S13" s="40"/>
+      <c r="T13" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U13" s="41"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" s="33">
+        <v>7</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="37"/>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="R14" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S14" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="T14" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U14" s="75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" s="33">
+        <v>8</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="K15" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="L15" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="M15" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" s="33">
+        <v>9</v>
+      </c>
+      <c r="B16" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="L16" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="P16" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="40"/>
+      <c r="S16" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="T16" s="40"/>
+      <c r="U16" s="41"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" s="33">
+        <v>10</v>
+      </c>
+      <c r="B17" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="37"/>
+      <c r="K17" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="37"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="40"/>
+      <c r="U17" s="75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18" s="33">
+        <v>11</v>
+      </c>
+      <c r="B18" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="N18" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="O18" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="P18" s="76" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="77" t="s">
+        <v>4</v>
+      </c>
+      <c r="R18" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S18" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="T18" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U18" s="75" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="O19" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P19" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="T19" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U19" s="78"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A20" s="33">
+        <v>13</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="37"/>
+      <c r="K20" s="37"/>
+      <c r="L20" s="37"/>
+      <c r="M20" s="37"/>
+      <c r="N20" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="O20" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="P20" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="R20" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="S20" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="T20" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="U20" s="113" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" s="33">
+        <v>14</v>
+      </c>
+      <c r="B21" s="42"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="37"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="37"/>
+      <c r="K21" s="37"/>
+      <c r="L21" s="37"/>
+      <c r="M21" s="37"/>
+      <c r="N21" s="37"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="41"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A22" s="33">
+        <v>15</v>
+      </c>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="37"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="37"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="39"/>
+      <c r="R22" s="40"/>
+      <c r="S22" s="40"/>
+      <c r="T22" s="40"/>
+      <c r="U22" s="41"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A23" s="33">
+        <v>16</v>
+      </c>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="37"/>
+      <c r="N23" s="37"/>
+      <c r="O23" s="37"/>
+      <c r="P23" s="38"/>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="40"/>
+      <c r="S23" s="40"/>
+      <c r="T23" s="40"/>
+      <c r="U23" s="41"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A24" s="44">
+        <v>17</v>
+      </c>
+      <c r="B24" s="45"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
+      <c r="N24" s="48"/>
+      <c r="O24" s="48"/>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="50"/>
+      <c r="R24" s="51"/>
+      <c r="S24" s="51"/>
+      <c r="T24" s="51"/>
+      <c r="U24" s="52"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A25" s="53"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="98" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="87" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="87" t="s">
+        <v>9</v>
+      </c>
+      <c r="H25" s="87" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="87" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="87" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="87" t="s">
+        <v>13</v>
+      </c>
+      <c r="L25" s="87" t="s">
+        <v>14</v>
+      </c>
+      <c r="M25" s="87" t="s">
+        <v>15</v>
+      </c>
+      <c r="N25" s="87" t="s">
+        <v>16</v>
+      </c>
+      <c r="O25" s="87" t="s">
+        <v>17</v>
+      </c>
+      <c r="P25" s="89" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q25" s="96" t="s">
+        <v>19</v>
+      </c>
+      <c r="R25" s="85" t="s">
+        <v>20</v>
+      </c>
+      <c r="S25" s="85" t="s">
+        <v>21</v>
+      </c>
+      <c r="T25" s="85" t="s">
+        <v>30</v>
+      </c>
+      <c r="U25" s="94" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="53"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="98"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="87"/>
+      <c r="I26" s="87"/>
+      <c r="J26" s="87"/>
+      <c r="K26" s="87"/>
+      <c r="L26" s="87"/>
+      <c r="M26" s="87"/>
+      <c r="N26" s="87"/>
+      <c r="O26" s="87"/>
+      <c r="P26" s="89"/>
+      <c r="Q26" s="96"/>
+      <c r="R26" s="85"/>
+      <c r="S26" s="85"/>
+      <c r="T26" s="85"/>
+      <c r="U26" s="94"/>
+    </row>
+    <row r="27" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="53"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="98"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="87"/>
+      <c r="J27" s="87"/>
+      <c r="K27" s="87"/>
+      <c r="L27" s="87"/>
+      <c r="M27" s="87"/>
+      <c r="N27" s="87"/>
+      <c r="O27" s="87"/>
+      <c r="P27" s="89"/>
+      <c r="Q27" s="96"/>
+      <c r="R27" s="85"/>
+      <c r="S27" s="85"/>
+      <c r="T27" s="85"/>
+      <c r="U27" s="94"/>
+    </row>
+    <row r="28" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="53"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="98"/>
+      <c r="F28" s="87"/>
+      <c r="G28" s="87"/>
+      <c r="H28" s="87"/>
+      <c r="I28" s="87"/>
+      <c r="J28" s="87"/>
+      <c r="K28" s="87"/>
+      <c r="L28" s="87"/>
+      <c r="M28" s="87"/>
+      <c r="N28" s="87"/>
+      <c r="O28" s="87"/>
+      <c r="P28" s="89"/>
+      <c r="Q28" s="96"/>
+      <c r="R28" s="85"/>
+      <c r="S28" s="85"/>
+      <c r="T28" s="85"/>
+      <c r="U28" s="94"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A29" s="53"/>
+      <c r="B29" s="54"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="98"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
+      <c r="H29" s="87"/>
+      <c r="I29" s="87"/>
+      <c r="J29" s="87"/>
+      <c r="K29" s="87"/>
+      <c r="L29" s="87"/>
+      <c r="M29" s="87"/>
+      <c r="N29" s="87"/>
+      <c r="O29" s="87"/>
+      <c r="P29" s="89"/>
+      <c r="Q29" s="96"/>
+      <c r="R29" s="85"/>
+      <c r="S29" s="85"/>
+      <c r="T29" s="85"/>
+      <c r="U29" s="94"/>
+    </row>
+    <row r="30" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="53"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="99"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="88"/>
+      <c r="H30" s="88"/>
+      <c r="I30" s="88"/>
+      <c r="J30" s="88"/>
+      <c r="K30" s="88"/>
+      <c r="L30" s="88"/>
+      <c r="M30" s="88"/>
+      <c r="N30" s="88"/>
+      <c r="O30" s="88"/>
+      <c r="P30" s="90"/>
+      <c r="Q30" s="97"/>
+      <c r="R30" s="86"/>
+      <c r="S30" s="86"/>
+      <c r="T30" s="86"/>
+      <c r="U30" s="95"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A31" s="112" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="92"/>
+      <c r="C31" s="92"/>
+      <c r="D31" s="92"/>
+      <c r="E31" s="92"/>
+      <c r="F31" s="92"/>
+      <c r="G31" s="92"/>
+      <c r="H31" s="92"/>
+      <c r="I31" s="92"/>
+      <c r="J31" s="92"/>
+      <c r="K31" s="92"/>
+      <c r="L31" s="92"/>
+      <c r="M31" s="92"/>
+      <c r="N31" s="92"/>
+      <c r="O31" s="92"/>
+      <c r="P31" s="92"/>
+      <c r="Q31" s="92"/>
+      <c r="R31" s="92"/>
+      <c r="S31" s="92"/>
+      <c r="T31" s="92"/>
+      <c r="U31" s="93"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A32" s="111" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="80"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="80"/>
+      <c r="F32" s="80"/>
+      <c r="G32" s="80"/>
+      <c r="H32" s="80"/>
+      <c r="I32" s="80"/>
+      <c r="J32" s="80"/>
+      <c r="K32" s="80"/>
+      <c r="L32" s="80"/>
+      <c r="M32" s="80"/>
+      <c r="N32" s="80"/>
+      <c r="O32" s="80"/>
+      <c r="P32" s="80"/>
+      <c r="Q32" s="80"/>
+      <c r="R32" s="80"/>
+      <c r="S32" s="80"/>
+      <c r="T32" s="80"/>
+      <c r="U32" s="81"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A33" s="111" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="80"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="80"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="80"/>
+      <c r="H33" s="80"/>
+      <c r="I33" s="80"/>
+      <c r="J33" s="80"/>
+      <c r="K33" s="80"/>
+      <c r="L33" s="80"/>
+      <c r="M33" s="80"/>
+      <c r="N33" s="80"/>
+      <c r="O33" s="80"/>
+      <c r="P33" s="80"/>
+      <c r="Q33" s="80"/>
+      <c r="R33" s="80"/>
+      <c r="S33" s="80"/>
+      <c r="T33" s="80"/>
+      <c r="U33" s="81"/>
+    </row>
+    <row r="34" spans="1:21" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="83"/>
+      <c r="C34" s="83"/>
+      <c r="D34" s="83"/>
+      <c r="E34" s="83"/>
+      <c r="F34" s="83"/>
+      <c r="G34" s="83"/>
+      <c r="H34" s="83"/>
+      <c r="I34" s="83"/>
+      <c r="J34" s="83"/>
+      <c r="K34" s="83"/>
+      <c r="L34" s="83"/>
+      <c r="M34" s="83"/>
+      <c r="N34" s="83"/>
+      <c r="O34" s="83"/>
+      <c r="P34" s="83"/>
+      <c r="Q34" s="83"/>
+      <c r="R34" s="83"/>
+      <c r="S34" s="83"/>
+      <c r="T34" s="83"/>
+      <c r="U34" s="84"/>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A35" s="18"/>
@@ -6626,7 +8264,7 @@
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5:G5 I5:K5 M5:P5 P6 G6:L7 E8:F8 J8:L8 K11 P11 E11:G12 I12:L12 O12:P12 E13:J13 M13:P13 E14:H14 J14:N14 P14 N15:P15 E15:I16 M16:O16 E17:J17 L17:P17 E18:I18 K18:L18 E21:P24 E20:M20">
+  <conditionalFormatting sqref="F5:G5 I5:K5 M5:P5 P6 G6:L7 E8:F8 J8:L8 K11 E11:G12 I12:L12 P11:P12 E13:J13 M13:P13 E14:H14 J14:N14 P14 N15:P15 E15:I16 M16:N16 E17:J17 L17:P17 E18:I18 K18:L18 E20:M20 E21:P24">
     <cfRule type="cellIs" dxfId="11" priority="13" stopIfTrue="1" operator="equal">
       <formula>"S"</formula>
     </cfRule>

</xml_diff>